<commit_message>
U W H corner algs
</commit_message>
<xml_diff>
--- a/cube/data/3-style_data.xlsx
+++ b/cube/data/3-style_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\j_bou\Documents\Code\github.io\cube\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE0AD887-8180-4EC5-B198-BEB46F84B2E9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9B9A2C3-3530-4818-BADE-F8EB8DFC2091}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1005,6 +1005,19 @@
         </r>
       </text>
     </comment>
+    <comment ref="J23" authorId="1" shapeId="0" xr:uid="{97B3114B-4A17-4C08-8F1B-C42B34E80CB6}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>[U: [F', R U R2 U' R']]</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="O23" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-00004B000000}">
       <text>
         <r>
@@ -1140,7 +1153,7 @@
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
           </rPr>
-          <t>[R D' R’: [R'D R, U]]</t>
+          <t>[R D' R': [R' D R, U]]</t>
         </r>
       </text>
     </comment>
@@ -22856,10 +22869,10 @@
   <dimension ref="A1:Z36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="I8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="E8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="O21" sqref="O21"/>
+      <selection pane="bottomRight" activeCell="L30" sqref="L30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="19.5" customHeight="1"/>

</xml_diff>

<commit_message>
Words + G H S T R E Q F algs + controller fix
</commit_message>
<xml_diff>
--- a/cube/data/3-style_data.xlsx
+++ b/cube/data/3-style_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\j_bou\Documents\Code\github.io\cube\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9B9A2C3-3530-4818-BADE-F8EB8DFC2091}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF8CCA46-3601-43C1-AAB5-A645F8048999}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,6 +24,7 @@
     <sheet name="Obliques" sheetId="8" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -13491,6 +13492,13 @@
     <xf numFmtId="0" fontId="30" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -13499,13 +13507,6 @@
     </xf>
     <xf numFmtId="0" fontId="34" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -22869,10 +22870,10 @@
   <dimension ref="A1:Z36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="E8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="F7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L30" sqref="L30"/>
+      <selection pane="bottomRight" activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="19.5" customHeight="1"/>
@@ -24059,7 +24060,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H15" sqref="H15"/>
+      <selection pane="bottomRight" activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="19.5" customHeight="1"/>
@@ -25405,15 +25406,15 @@
     </row>
     <row r="27" spans="1:26" ht="19.5" customHeight="1">
       <c r="A27" s="46"/>
-      <c r="B27" s="126" t="s">
+      <c r="B27" s="129" t="s">
         <v>529</v>
       </c>
-      <c r="C27" s="125"/>
+      <c r="C27" s="128"/>
       <c r="D27" s="48"/>
-      <c r="E27" s="127" t="s">
+      <c r="E27" s="126" t="s">
         <v>529</v>
       </c>
-      <c r="F27" s="128"/>
+      <c r="F27" s="125"/>
       <c r="G27" s="48"/>
       <c r="H27" s="48"/>
       <c r="I27" s="48"/>
@@ -25440,15 +25441,15 @@
         <f>CONCATENATE(Key!C4, " / ", Key!S4)</f>
         <v>A / Q</v>
       </c>
-      <c r="B28" s="124" t="s">
+      <c r="B28" s="127" t="s">
         <v>534</v>
       </c>
-      <c r="C28" s="125"/>
+      <c r="C28" s="128"/>
       <c r="D28" s="48"/>
-      <c r="E28" s="129" t="s">
+      <c r="E28" s="124" t="s">
         <v>534</v>
       </c>
-      <c r="F28" s="128"/>
+      <c r="F28" s="125"/>
       <c r="G28" s="48"/>
       <c r="H28" s="48"/>
       <c r="I28" s="48"/>
@@ -25475,15 +25476,15 @@
         <f>CONCATENATE(Key!D4, " / ", Key!O4)</f>
         <v>B / M</v>
       </c>
-      <c r="B29" s="124" t="s">
+      <c r="B29" s="127" t="s">
         <v>535</v>
       </c>
-      <c r="C29" s="125"/>
+      <c r="C29" s="128"/>
       <c r="D29" s="48"/>
-      <c r="E29" s="129" t="s">
+      <c r="E29" s="124" t="s">
         <v>535</v>
       </c>
-      <c r="F29" s="128"/>
+      <c r="F29" s="125"/>
       <c r="G29" s="48"/>
       <c r="H29" s="48"/>
       <c r="I29" s="48"/>
@@ -25510,15 +25511,15 @@
         <f>CONCATENATE(Key!F4, " / ", Key!G4)</f>
         <v>D / E</v>
       </c>
-      <c r="B30" s="124" t="s">
+      <c r="B30" s="127" t="s">
         <v>538</v>
       </c>
-      <c r="C30" s="125"/>
+      <c r="C30" s="128"/>
       <c r="D30" s="48"/>
-      <c r="E30" s="129" t="s">
+      <c r="E30" s="124" t="s">
         <v>538</v>
       </c>
-      <c r="F30" s="128"/>
+      <c r="F30" s="125"/>
       <c r="G30" s="48"/>
       <c r="H30" s="48"/>
       <c r="I30" s="48"/>
@@ -25545,15 +25546,15 @@
         <f>CONCATENATE(Key!H4, " / ", Key!N4)</f>
         <v>F / L</v>
       </c>
-      <c r="B31" s="124" t="s">
+      <c r="B31" s="127" t="s">
         <v>539</v>
       </c>
-      <c r="C31" s="125"/>
+      <c r="C31" s="128"/>
       <c r="D31" s="48"/>
-      <c r="E31" s="129" t="s">
+      <c r="E31" s="124" t="s">
         <v>539</v>
       </c>
-      <c r="F31" s="128"/>
+      <c r="F31" s="125"/>
       <c r="G31" s="48"/>
       <c r="H31" s="48"/>
       <c r="I31" s="48"/>
@@ -25580,15 +25581,15 @@
         <f>CONCATENATE(Key!I4, " / ", Key!Z4)</f>
         <v>G / X</v>
       </c>
-      <c r="B32" s="124" t="s">
+      <c r="B32" s="127" t="s">
         <v>542</v>
       </c>
-      <c r="C32" s="125"/>
+      <c r="C32" s="128"/>
       <c r="D32" s="48"/>
-      <c r="E32" s="129" t="s">
+      <c r="E32" s="124" t="s">
         <v>542</v>
       </c>
-      <c r="F32" s="128"/>
+      <c r="F32" s="125"/>
       <c r="G32" s="48"/>
       <c r="H32" s="48"/>
       <c r="I32" s="48"/>
@@ -25615,15 +25616,15 @@
         <f>CONCATENATE(Key!J4, " / ", Key!T4)</f>
         <v>H / R</v>
       </c>
-      <c r="B33" s="124" t="s">
+      <c r="B33" s="127" t="s">
         <v>545</v>
       </c>
-      <c r="C33" s="125"/>
+      <c r="C33" s="128"/>
       <c r="D33" s="48"/>
-      <c r="E33" s="129" t="s">
+      <c r="E33" s="124" t="s">
         <v>545</v>
       </c>
-      <c r="F33" s="128"/>
+      <c r="F33" s="125"/>
       <c r="G33" s="48"/>
       <c r="H33" s="48"/>
       <c r="I33" s="48"/>
@@ -25650,15 +25651,15 @@
         <f>CONCATENATE(Key!L4, " / ", Key!R4)</f>
         <v>J / P</v>
       </c>
-      <c r="B34" s="124" t="s">
+      <c r="B34" s="127" t="s">
         <v>550</v>
       </c>
-      <c r="C34" s="125"/>
+      <c r="C34" s="128"/>
       <c r="D34" s="48"/>
-      <c r="E34" s="129" t="s">
+      <c r="E34" s="124" t="s">
         <v>550</v>
       </c>
-      <c r="F34" s="128"/>
+      <c r="F34" s="125"/>
       <c r="G34" s="48"/>
       <c r="H34" s="48"/>
       <c r="I34" s="48"/>
@@ -25685,15 +25686,15 @@
         <f>CONCATENATE(Key!M4, " / ", Key!W4)</f>
         <v>K / U</v>
       </c>
-      <c r="B35" s="124" t="s">
+      <c r="B35" s="127" t="s">
         <v>551</v>
       </c>
-      <c r="C35" s="125"/>
+      <c r="C35" s="128"/>
       <c r="D35" s="48"/>
-      <c r="E35" s="129" t="s">
+      <c r="E35" s="124" t="s">
         <v>551</v>
       </c>
-      <c r="F35" s="128"/>
+      <c r="F35" s="125"/>
       <c r="G35" s="48"/>
       <c r="H35" s="48"/>
       <c r="I35" s="48"/>
@@ -25720,15 +25721,15 @@
         <f>CONCATENATE(Key!P4, " / ", Key!V4)</f>
         <v>N / T</v>
       </c>
-      <c r="B36" s="124" t="s">
+      <c r="B36" s="127" t="s">
         <v>552</v>
       </c>
-      <c r="C36" s="125"/>
+      <c r="C36" s="128"/>
       <c r="D36" s="48"/>
-      <c r="E36" s="129" t="s">
+      <c r="E36" s="124" t="s">
         <v>552</v>
       </c>
-      <c r="F36" s="128"/>
+      <c r="F36" s="125"/>
       <c r="G36" s="48"/>
       <c r="H36" s="48"/>
       <c r="I36" s="48"/>
@@ -25755,15 +25756,15 @@
         <f>CONCATENATE(Key!Q4, " / ", Key!X4)</f>
         <v>O / V</v>
       </c>
-      <c r="B37" s="124" t="s">
+      <c r="B37" s="127" t="s">
         <v>553</v>
       </c>
-      <c r="C37" s="125"/>
+      <c r="C37" s="128"/>
       <c r="D37" s="48"/>
-      <c r="E37" s="129" t="s">
+      <c r="E37" s="124" t="s">
         <v>553</v>
       </c>
-      <c r="F37" s="128"/>
+      <c r="F37" s="125"/>
       <c r="G37" s="48"/>
       <c r="H37" s="48"/>
       <c r="I37" s="48"/>
@@ -25790,15 +25791,15 @@
         <f>CONCATENATE(Key!U4, " / ", Key!Y4)</f>
         <v>S / W</v>
       </c>
-      <c r="B38" s="124" t="s">
+      <c r="B38" s="127" t="s">
         <v>554</v>
       </c>
-      <c r="C38" s="125"/>
+      <c r="C38" s="128"/>
       <c r="D38" s="48"/>
-      <c r="E38" s="129" t="s">
+      <c r="E38" s="124" t="s">
         <v>554</v>
       </c>
-      <c r="F38" s="128"/>
+      <c r="F38" s="125"/>
       <c r="G38" s="48"/>
       <c r="H38" s="48"/>
       <c r="I38" s="48"/>
@@ -25850,6 +25851,23 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="E31:F31"/>
     <mergeCell ref="E37:F37"/>
     <mergeCell ref="E38:F38"/>
     <mergeCell ref="E32:F32"/>
@@ -25857,23 +25875,6 @@
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B31:C31"/>
   </mergeCells>
   <conditionalFormatting sqref="B1:E1 A2:A5">
     <cfRule type="expression" dxfId="155" priority="2">
@@ -30258,11 +30259,13 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="B50:E50"/>
-    <mergeCell ref="B51:E51"/>
-    <mergeCell ref="B48:E48"/>
-    <mergeCell ref="B49:E49"/>
-    <mergeCell ref="B47:E47"/>
+    <mergeCell ref="B33:E33"/>
+    <mergeCell ref="B32:E32"/>
+    <mergeCell ref="B28:E28"/>
+    <mergeCell ref="B27:E27"/>
+    <mergeCell ref="B29:E29"/>
+    <mergeCell ref="B30:E30"/>
+    <mergeCell ref="B31:E31"/>
     <mergeCell ref="B44:E44"/>
     <mergeCell ref="B45:E45"/>
     <mergeCell ref="B46:E46"/>
@@ -30276,13 +30279,11 @@
     <mergeCell ref="B39:E39"/>
     <mergeCell ref="B38:E38"/>
     <mergeCell ref="B41:E41"/>
-    <mergeCell ref="B33:E33"/>
-    <mergeCell ref="B32:E32"/>
-    <mergeCell ref="B28:E28"/>
-    <mergeCell ref="B27:E27"/>
-    <mergeCell ref="B29:E29"/>
-    <mergeCell ref="B30:E30"/>
-    <mergeCell ref="B31:E31"/>
+    <mergeCell ref="B50:E50"/>
+    <mergeCell ref="B51:E51"/>
+    <mergeCell ref="B48:E48"/>
+    <mergeCell ref="B49:E49"/>
+    <mergeCell ref="B47:E47"/>
   </mergeCells>
   <conditionalFormatting sqref="B1:E1 A2:A5">
     <cfRule type="expression" dxfId="92" priority="1">

</xml_diff>

<commit_message>
Another words and edge alg update
</commit_message>
<xml_diff>
--- a/cube/data/3-style_data.xlsx
+++ b/cube/data/3-style_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\j_bou\Documents\Code\github.io\cube\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B9752D6-A7B7-41BB-A036-D420B399A1BC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{849DD64E-1419-46B3-83FD-B34163364A4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1860" yWindow="1860" windowWidth="21600" windowHeight="11265" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Letter Pair Words" sheetId="9" r:id="rId1"/>
@@ -10971,9 +10971,6 @@
     <t>Ed</t>
   </si>
   <si>
-    <t>food</t>
-  </si>
-  <si>
     <t>God</t>
   </si>
   <si>
@@ -11208,9 +11205,6 @@
     <t>mud</t>
   </si>
   <si>
-    <t>Maaf</t>
-  </si>
-  <si>
     <t>knife</t>
   </si>
   <si>
@@ -11271,9 +11265,6 @@
     <t>squeedge</t>
   </si>
   <si>
-    <t>wage</t>
-  </si>
-  <si>
     <t>jerk</t>
   </si>
   <si>
@@ -11421,9 +11412,6 @@
     <t>Xev</t>
   </si>
   <si>
-    <t>Gab</t>
-  </si>
-  <si>
     <t>[F', L S L']</t>
   </si>
   <si>
@@ -11616,9 +11604,6 @@
     <t>Aj</t>
   </si>
   <si>
-    <t>bœuf</t>
-  </si>
-  <si>
     <t>bûche</t>
   </si>
   <si>
@@ -11640,9 +11625,6 @@
     <t>eb</t>
   </si>
   <si>
-    <t>ailes</t>
-  </si>
-  <si>
     <t>help</t>
   </si>
   <si>
@@ -11856,9 +11838,6 @@
     <t>mate</t>
   </si>
   <si>
-    <t>mal</t>
-  </si>
-  <si>
     <t>Na</t>
   </si>
   <si>
@@ -11949,18 +11928,12 @@
     <t>Pot</t>
   </si>
   <si>
-    <t>pawn</t>
-  </si>
-  <si>
     <t>prize</t>
   </si>
   <si>
     <t>Page</t>
   </si>
   <si>
-    <t>bench</t>
-  </si>
-  <si>
     <t>bee</t>
   </si>
   <si>
@@ -12006,9 +11979,6 @@
     <t>run</t>
   </si>
   <si>
-    <t>Raxxx</t>
-  </si>
-  <si>
     <t>Gates</t>
   </si>
   <si>
@@ -12054,9 +12024,6 @@
     <t>Smurf</t>
   </si>
   <si>
-    <t>singe</t>
-  </si>
-  <si>
     <t>Mahj</t>
   </si>
   <si>
@@ -12144,9 +12111,6 @@
     <t>zen</t>
   </si>
   <si>
-    <t>Zef</t>
-  </si>
-  <si>
     <t>Zhao</t>
   </si>
   <si>
@@ -12168,9 +12132,6 @@
     <t>zest</t>
   </si>
   <si>
-    <t>Zur</t>
-  </si>
-  <si>
     <t>zit</t>
   </si>
   <si>
@@ -12228,9 +12189,6 @@
     <t>Jean</t>
   </si>
   <si>
-    <t>whip</t>
-  </si>
-  <si>
     <t>Louis</t>
   </si>
   <si>
@@ -12288,9 +12246,6 @@
     <t>quartz</t>
   </si>
   <si>
-    <t>quad</t>
-  </si>
-  <si>
     <t>quench</t>
   </si>
   <si>
@@ -12369,18 +12324,12 @@
     <t>Ritz</t>
   </si>
   <si>
-    <t>knit</t>
-  </si>
-  <si>
     <t>tatt</t>
   </si>
   <si>
     <t>son</t>
   </si>
   <si>
-    <t>Op</t>
-  </si>
-  <si>
     <t>ninj</t>
   </si>
   <si>
@@ -12417,9 +12366,6 @@
     <t>rêve</t>
   </si>
   <si>
-    <t>sleigh</t>
-  </si>
-  <si>
     <t>Leg</t>
   </si>
   <si>
@@ -12447,9 +12393,6 @@
     <t>Eur</t>
   </si>
   <si>
-    <t>Flash</t>
-  </si>
-  <si>
     <t>hov</t>
   </si>
   <si>
@@ -12459,9 +12402,6 @@
     <t>Alp</t>
   </si>
   <si>
-    <t>bell</t>
-  </si>
-  <si>
     <t>boom</t>
   </si>
   <si>
@@ -12504,9 +12444,6 @@
     <t>quai</t>
   </si>
   <si>
-    <t>rook</t>
-  </si>
-  <si>
     <t>Thor</t>
   </si>
   <si>
@@ -12529,6 +12466,69 @@
   </si>
   <si>
     <t>Om</t>
+  </si>
+  <si>
+    <t>grab</t>
+  </si>
+  <si>
+    <t>maf</t>
+  </si>
+  <si>
+    <t>Mal</t>
+  </si>
+  <si>
+    <t>El</t>
+  </si>
+  <si>
+    <t>flood</t>
+  </si>
+  <si>
+    <t>cop</t>
+  </si>
+  <si>
+    <t>flash</t>
+  </si>
+  <si>
+    <t>Rax</t>
+  </si>
+  <si>
+    <t>wedge</t>
+  </si>
+  <si>
+    <t>Zeph</t>
+  </si>
+  <si>
+    <t>Zerg</t>
+  </si>
+  <si>
+    <t>quid</t>
+  </si>
+  <si>
+    <t>blood</t>
+  </si>
+  <si>
+    <t>Seg</t>
+  </si>
+  <si>
+    <t>slay</t>
+  </si>
+  <si>
+    <t>Beach</t>
+  </si>
+  <si>
+    <t>baffe</t>
+  </si>
+  <si>
+    <t>Wa</t>
+  </si>
+  <si>
+    <t>rack</t>
+  </si>
+  <si>
+    <t>pow</t>
+  </si>
+  <si>
+    <t>Nat</t>
   </si>
 </sst>
 </file>
@@ -15683,8 +15683,8 @@
   </sheetPr>
   <dimension ref="B1:AW51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L41" sqref="L41"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="U45" sqref="U45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -15793,7 +15793,7 @@
         <v>1826</v>
       </c>
       <c r="H3" s="75" t="s">
-        <v>2229</v>
+        <v>2218</v>
       </c>
       <c r="I3" s="72"/>
       <c r="J3" s="76"/>
@@ -15807,7 +15807,7 @@
         <v>1826</v>
       </c>
       <c r="P3" s="71" t="s">
-        <v>2122</v>
+        <v>2116</v>
       </c>
       <c r="Q3" s="72"/>
       <c r="R3" s="69" t="s">
@@ -15827,7 +15827,7 @@
         <v>1826</v>
       </c>
       <c r="X3" s="71" t="s">
-        <v>1906</v>
+        <v>1905</v>
       </c>
       <c r="Y3" s="72"/>
       <c r="Z3" s="69" t="s">
@@ -15837,7 +15837,7 @@
         <v>1826</v>
       </c>
       <c r="AB3" s="71" t="s">
-        <v>2146</v>
+        <v>2140</v>
       </c>
       <c r="AC3" s="72"/>
       <c r="AD3" s="69" t="s">
@@ -15847,7 +15847,7 @@
         <v>1826</v>
       </c>
       <c r="AF3" s="71" t="s">
-        <v>2107</v>
+        <v>2101</v>
       </c>
       <c r="AG3" s="72"/>
       <c r="AH3" s="69" t="s">
@@ -15867,7 +15867,7 @@
         <v>1826</v>
       </c>
       <c r="AN3" s="71" t="s">
-        <v>2132</v>
+        <v>2126</v>
       </c>
       <c r="AO3" s="72"/>
       <c r="AP3" s="69" t="s">
@@ -15887,7 +15887,7 @@
         <v>1826</v>
       </c>
       <c r="AV3" s="71" t="s">
-        <v>2280</v>
+        <v>2267</v>
       </c>
     </row>
     <row r="4" spans="2:48">
@@ -15916,7 +15916,7 @@
         <v>1827</v>
       </c>
       <c r="P4" s="84" t="s">
-        <v>2328</v>
+        <v>2313</v>
       </c>
       <c r="Q4" s="72"/>
       <c r="R4" s="82" t="s">
@@ -15926,7 +15926,7 @@
         <v>1827</v>
       </c>
       <c r="T4" s="84" t="s">
-        <v>2088</v>
+        <v>2083</v>
       </c>
       <c r="U4" s="72"/>
       <c r="V4" s="82" t="s">
@@ -15946,7 +15946,7 @@
         <v>1827</v>
       </c>
       <c r="AB4" s="84" t="s">
-        <v>2016</v>
+        <v>2365</v>
       </c>
       <c r="AC4" s="72"/>
       <c r="AD4" s="82" t="s">
@@ -15956,7 +15956,7 @@
         <v>1827</v>
       </c>
       <c r="AF4" s="84" t="s">
-        <v>2125</v>
+        <v>2119</v>
       </c>
       <c r="AG4" s="72"/>
       <c r="AH4" s="82" t="s">
@@ -15966,7 +15966,7 @@
         <v>1827</v>
       </c>
       <c r="AJ4" s="84" t="s">
-        <v>2045</v>
+        <v>2041</v>
       </c>
       <c r="AK4" s="72"/>
       <c r="AL4" s="82" t="s">
@@ -15976,7 +15976,7 @@
         <v>1827</v>
       </c>
       <c r="AN4" s="84" t="s">
-        <v>2350</v>
+        <v>2332</v>
       </c>
       <c r="AO4" s="72"/>
       <c r="AP4" s="82" t="s">
@@ -15986,7 +15986,7 @@
         <v>1827</v>
       </c>
       <c r="AR4" s="84" t="s">
-        <v>2144</v>
+        <v>2138</v>
       </c>
       <c r="AS4" s="72"/>
       <c r="AT4" s="82" t="s">
@@ -15996,7 +15996,7 @@
         <v>1827</v>
       </c>
       <c r="AV4" s="84" t="s">
-        <v>2156</v>
+        <v>2150</v>
       </c>
     </row>
     <row r="5" spans="2:48">
@@ -16066,7 +16066,7 @@
         <v>1829</v>
       </c>
       <c r="H6" s="84" t="s">
-        <v>2321</v>
+        <v>2306</v>
       </c>
       <c r="I6" s="72"/>
       <c r="J6" s="85"/>
@@ -16094,7 +16094,7 @@
         <v>1829</v>
       </c>
       <c r="X6" s="84" t="s">
-        <v>1866</v>
+        <v>2369</v>
       </c>
       <c r="Y6" s="72"/>
       <c r="Z6" s="82" t="s">
@@ -16104,7 +16104,7 @@
         <v>1829</v>
       </c>
       <c r="AB6" s="84" t="s">
-        <v>1867</v>
+        <v>1866</v>
       </c>
       <c r="AC6" s="72"/>
       <c r="AD6" s="82" t="s">
@@ -16114,7 +16114,7 @@
         <v>1829</v>
       </c>
       <c r="AF6" s="84" t="s">
-        <v>1868</v>
+        <v>1867</v>
       </c>
       <c r="AG6" s="72"/>
       <c r="AH6" s="85"/>
@@ -16128,7 +16128,7 @@
         <v>1829</v>
       </c>
       <c r="AN6" s="84" t="s">
-        <v>2367</v>
+        <v>2347</v>
       </c>
       <c r="AO6" s="72"/>
       <c r="AP6" s="82" t="s">
@@ -16138,7 +16138,7 @@
         <v>1829</v>
       </c>
       <c r="AR6" s="84" t="s">
-        <v>1869</v>
+        <v>1868</v>
       </c>
       <c r="AS6" s="72"/>
       <c r="AT6" s="82" t="s">
@@ -16148,7 +16148,7 @@
         <v>1829</v>
       </c>
       <c r="AV6" s="84" t="s">
-        <v>1870</v>
+        <v>1869</v>
       </c>
     </row>
     <row r="7" spans="2:48">
@@ -16159,7 +16159,7 @@
         <v>1830</v>
       </c>
       <c r="D7" s="84" t="s">
-        <v>2034</v>
+        <v>2030</v>
       </c>
       <c r="E7" s="72"/>
       <c r="F7" s="82" t="s">
@@ -16169,7 +16169,7 @@
         <v>1830</v>
       </c>
       <c r="H7" s="84" t="s">
-        <v>2195</v>
+        <v>2380</v>
       </c>
       <c r="I7" s="72"/>
       <c r="J7" s="85"/>
@@ -16183,7 +16183,7 @@
         <v>1830</v>
       </c>
       <c r="P7" s="84" t="s">
-        <v>2083</v>
+        <v>2078</v>
       </c>
       <c r="Q7" s="72"/>
       <c r="R7" s="82"/>
@@ -16197,7 +16197,7 @@
         <v>1830</v>
       </c>
       <c r="X7" s="81" t="s">
-        <v>2095</v>
+        <v>2089</v>
       </c>
       <c r="Y7" s="72"/>
       <c r="Z7" s="82" t="s">
@@ -16207,7 +16207,7 @@
         <v>1830</v>
       </c>
       <c r="AB7" s="84" t="s">
-        <v>1871</v>
+        <v>1870</v>
       </c>
       <c r="AC7" s="72"/>
       <c r="AD7" s="82" t="s">
@@ -16217,7 +16217,7 @@
         <v>1830</v>
       </c>
       <c r="AF7" s="84" t="s">
-        <v>1899</v>
+        <v>1898</v>
       </c>
       <c r="AG7" s="72"/>
       <c r="AH7" s="82" t="s">
@@ -16227,7 +16227,7 @@
         <v>1830</v>
       </c>
       <c r="AJ7" s="84" t="s">
-        <v>1872</v>
+        <v>1871</v>
       </c>
       <c r="AK7" s="72"/>
       <c r="AL7" s="82" t="s">
@@ -16237,7 +16237,7 @@
         <v>1830</v>
       </c>
       <c r="AN7" s="84" t="s">
-        <v>2284</v>
+        <v>2271</v>
       </c>
       <c r="AO7" s="72"/>
       <c r="AP7" s="82" t="s">
@@ -16247,7 +16247,7 @@
         <v>1830</v>
       </c>
       <c r="AR7" s="84" t="s">
-        <v>1873</v>
+        <v>1872</v>
       </c>
       <c r="AS7" s="72"/>
       <c r="AT7" s="82" t="s">
@@ -16257,7 +16257,7 @@
         <v>1830</v>
       </c>
       <c r="AV7" s="84" t="s">
-        <v>2147</v>
+        <v>2141</v>
       </c>
     </row>
     <row r="8" spans="2:48">
@@ -16268,7 +16268,7 @@
         <v>1831</v>
       </c>
       <c r="D8" s="84" t="s">
-        <v>2360</v>
+        <v>2341</v>
       </c>
       <c r="E8" s="72"/>
       <c r="F8" s="82" t="s">
@@ -16278,7 +16278,7 @@
         <v>1831</v>
       </c>
       <c r="H8" s="84" t="s">
-        <v>2081</v>
+        <v>2381</v>
       </c>
       <c r="I8" s="72"/>
       <c r="J8" s="85"/>
@@ -16292,7 +16292,7 @@
         <v>1831</v>
       </c>
       <c r="P8" s="84" t="s">
-        <v>2084</v>
+        <v>2079</v>
       </c>
       <c r="Q8" s="72"/>
       <c r="R8" s="79" t="s">
@@ -16302,7 +16302,7 @@
         <v>1831</v>
       </c>
       <c r="T8" s="81" t="s">
-        <v>1874</v>
+        <v>1873</v>
       </c>
       <c r="U8" s="72"/>
       <c r="V8" s="82"/>
@@ -16316,7 +16316,7 @@
         <v>1831</v>
       </c>
       <c r="AB8" s="84" t="s">
-        <v>1875</v>
+        <v>1874</v>
       </c>
       <c r="AC8" s="72"/>
       <c r="AD8" s="82" t="s">
@@ -16326,7 +16326,7 @@
         <v>1831</v>
       </c>
       <c r="AF8" s="84" t="s">
-        <v>2108</v>
+        <v>2102</v>
       </c>
       <c r="AG8" s="72"/>
       <c r="AH8" s="85"/>
@@ -16340,7 +16340,7 @@
         <v>1831</v>
       </c>
       <c r="AN8" s="84" t="s">
-        <v>1876</v>
+        <v>1875</v>
       </c>
       <c r="AO8" s="72"/>
       <c r="AP8" s="82" t="s">
@@ -16350,7 +16350,7 @@
         <v>1831</v>
       </c>
       <c r="AR8" s="84" t="s">
-        <v>1947</v>
+        <v>1945</v>
       </c>
       <c r="AS8" s="72"/>
       <c r="AT8" s="82" t="s">
@@ -16360,7 +16360,7 @@
         <v>1831</v>
       </c>
       <c r="AV8" s="84" t="s">
-        <v>1877</v>
+        <v>1876</v>
       </c>
     </row>
     <row r="9" spans="2:48">
@@ -16371,7 +16371,7 @@
         <v>1832</v>
       </c>
       <c r="D9" s="84" t="s">
-        <v>2079</v>
+        <v>2075</v>
       </c>
       <c r="E9" s="72"/>
       <c r="F9" s="82" t="s">
@@ -16381,7 +16381,7 @@
         <v>1832</v>
       </c>
       <c r="H9" s="84" t="s">
-        <v>2023</v>
+        <v>2019</v>
       </c>
       <c r="I9" s="72"/>
       <c r="J9" s="85"/>
@@ -16395,7 +16395,7 @@
         <v>1832</v>
       </c>
       <c r="P9" s="84" t="s">
-        <v>1878</v>
+        <v>1877</v>
       </c>
       <c r="Q9" s="72"/>
       <c r="R9" s="82" t="s">
@@ -16405,7 +16405,7 @@
         <v>1832</v>
       </c>
       <c r="T9" s="84" t="s">
-        <v>1879</v>
+        <v>1878</v>
       </c>
       <c r="U9" s="72"/>
       <c r="V9" s="82" t="s">
@@ -16415,7 +16415,7 @@
         <v>1832</v>
       </c>
       <c r="X9" s="84" t="s">
-        <v>1880</v>
+        <v>1879</v>
       </c>
       <c r="Y9" s="72"/>
       <c r="Z9" s="82"/>
@@ -16429,7 +16429,7 @@
         <v>1832</v>
       </c>
       <c r="AF9" s="81" t="s">
-        <v>1881</v>
+        <v>1880</v>
       </c>
       <c r="AG9" s="72"/>
       <c r="AH9" s="82" t="s">
@@ -16439,7 +16439,7 @@
         <v>1832</v>
       </c>
       <c r="AJ9" s="84" t="s">
-        <v>2269</v>
+        <v>2256</v>
       </c>
       <c r="AK9" s="72"/>
       <c r="AL9" s="82" t="s">
@@ -16449,7 +16449,7 @@
         <v>1832</v>
       </c>
       <c r="AN9" s="84" t="s">
-        <v>1882</v>
+        <v>1881</v>
       </c>
       <c r="AO9" s="72"/>
       <c r="AP9" s="82" t="s">
@@ -16459,7 +16459,7 @@
         <v>1832</v>
       </c>
       <c r="AR9" s="84" t="s">
-        <v>2135</v>
+        <v>2129</v>
       </c>
       <c r="AS9" s="72"/>
       <c r="AT9" s="82" t="s">
@@ -16469,7 +16469,7 @@
         <v>1832</v>
       </c>
       <c r="AV9" s="84" t="s">
-        <v>2349</v>
+        <v>2331</v>
       </c>
     </row>
     <row r="10" spans="2:48">
@@ -16480,7 +16480,7 @@
         <v>1833</v>
       </c>
       <c r="D10" s="84" t="s">
-        <v>2353</v>
+        <v>2335</v>
       </c>
       <c r="E10" s="72"/>
       <c r="F10" s="82" t="s">
@@ -16490,7 +16490,7 @@
         <v>1833</v>
       </c>
       <c r="H10" s="84" t="s">
-        <v>2082</v>
+        <v>2077</v>
       </c>
       <c r="I10" s="72"/>
       <c r="J10" s="85"/>
@@ -16504,7 +16504,7 @@
         <v>1833</v>
       </c>
       <c r="P10" s="84" t="s">
-        <v>2121</v>
+        <v>2115</v>
       </c>
       <c r="Q10" s="72"/>
       <c r="R10" s="82" t="s">
@@ -16514,7 +16514,7 @@
         <v>1833</v>
       </c>
       <c r="T10" s="84" t="s">
-        <v>1883</v>
+        <v>1882</v>
       </c>
       <c r="U10" s="72"/>
       <c r="V10" s="82" t="s">
@@ -16524,7 +16524,7 @@
         <v>1833</v>
       </c>
       <c r="X10" s="84" t="s">
-        <v>2358</v>
+        <v>2371</v>
       </c>
       <c r="Y10" s="72"/>
       <c r="Z10" s="79" t="s">
@@ -16534,7 +16534,7 @@
         <v>1833</v>
       </c>
       <c r="AB10" s="81" t="s">
-        <v>1884</v>
+        <v>1883</v>
       </c>
       <c r="AC10" s="72"/>
       <c r="AD10" s="82"/>
@@ -16548,7 +16548,7 @@
         <v>1833</v>
       </c>
       <c r="AJ10" s="84" t="s">
-        <v>2126</v>
+        <v>2120</v>
       </c>
       <c r="AK10" s="72"/>
       <c r="AL10" s="82" t="s">
@@ -16558,7 +16558,7 @@
         <v>1833</v>
       </c>
       <c r="AN10" s="84" t="s">
-        <v>2283</v>
+        <v>2270</v>
       </c>
       <c r="AO10" s="72"/>
       <c r="AP10" s="82" t="s">
@@ -16568,7 +16568,7 @@
         <v>1833</v>
       </c>
       <c r="AR10" s="84" t="s">
-        <v>1969</v>
+        <v>1966</v>
       </c>
       <c r="AS10" s="72"/>
       <c r="AT10" s="82" t="s">
@@ -16578,7 +16578,7 @@
         <v>1833</v>
       </c>
       <c r="AV10" s="84" t="s">
-        <v>1886</v>
+        <v>1885</v>
       </c>
     </row>
     <row r="11" spans="2:48">
@@ -16589,7 +16589,7 @@
         <v>1834</v>
       </c>
       <c r="D11" s="84" t="s">
-        <v>2278</v>
+        <v>2265</v>
       </c>
       <c r="E11" s="72"/>
       <c r="F11" s="82" t="s">
@@ -16599,7 +16599,7 @@
         <v>1834</v>
       </c>
       <c r="H11" s="84" t="s">
-        <v>2196</v>
+        <v>2187</v>
       </c>
       <c r="I11" s="72"/>
       <c r="J11" s="85"/>
@@ -16617,7 +16617,7 @@
         <v>1834</v>
       </c>
       <c r="T11" s="84" t="s">
-        <v>2142</v>
+        <v>2136</v>
       </c>
       <c r="U11" s="72"/>
       <c r="V11" s="85"/>
@@ -16631,7 +16631,7 @@
         <v>1834</v>
       </c>
       <c r="AB11" s="84" t="s">
-        <v>2100</v>
+        <v>2094</v>
       </c>
       <c r="AC11" s="72"/>
       <c r="AD11" s="82" t="s">
@@ -16641,7 +16641,7 @@
         <v>1834</v>
       </c>
       <c r="AF11" s="84" t="s">
-        <v>1962</v>
+        <v>1960</v>
       </c>
       <c r="AG11" s="72"/>
       <c r="AH11" s="82"/>
@@ -16659,7 +16659,7 @@
         <v>1834</v>
       </c>
       <c r="AR11" s="84" t="s">
-        <v>1887</v>
+        <v>1886</v>
       </c>
       <c r="AS11" s="72"/>
       <c r="AT11" s="82" t="s">
@@ -16669,7 +16669,7 @@
         <v>1834</v>
       </c>
       <c r="AV11" s="84" t="s">
-        <v>2148</v>
+        <v>2142</v>
       </c>
     </row>
     <row r="12" spans="2:48">
@@ -16680,7 +16680,7 @@
         <v>1835</v>
       </c>
       <c r="D12" s="84" t="s">
-        <v>2080</v>
+        <v>2076</v>
       </c>
       <c r="E12" s="72"/>
       <c r="F12" s="82" t="s">
@@ -16690,7 +16690,7 @@
         <v>1835</v>
       </c>
       <c r="H12" s="84" t="s">
-        <v>2288</v>
+        <v>2274</v>
       </c>
       <c r="I12" s="72"/>
       <c r="J12" s="85"/>
@@ -16704,7 +16704,7 @@
         <v>1835</v>
       </c>
       <c r="P12" s="84" t="s">
-        <v>1888</v>
+        <v>1887</v>
       </c>
       <c r="Q12" s="72"/>
       <c r="R12" s="82" t="s">
@@ -16714,7 +16714,7 @@
         <v>1835</v>
       </c>
       <c r="T12" s="84" t="s">
-        <v>1889</v>
+        <v>1888</v>
       </c>
       <c r="U12" s="72"/>
       <c r="V12" s="82" t="s">
@@ -16724,7 +16724,7 @@
         <v>1835</v>
       </c>
       <c r="X12" s="84" t="s">
-        <v>2096</v>
+        <v>2090</v>
       </c>
       <c r="Y12" s="72"/>
       <c r="Z12" s="82" t="s">
@@ -16734,7 +16734,7 @@
         <v>1835</v>
       </c>
       <c r="AB12" s="84" t="s">
-        <v>2101</v>
+        <v>2095</v>
       </c>
       <c r="AC12" s="72"/>
       <c r="AD12" s="82" t="s">
@@ -16744,7 +16744,7 @@
         <v>1835</v>
       </c>
       <c r="AF12" s="84" t="s">
-        <v>1890</v>
+        <v>1889</v>
       </c>
       <c r="AG12" s="72"/>
       <c r="AH12" s="85"/>
@@ -16762,7 +16762,7 @@
         <v>1835</v>
       </c>
       <c r="AR12" s="84" t="s">
-        <v>2021</v>
+        <v>2017</v>
       </c>
       <c r="AS12" s="72"/>
       <c r="AT12" s="82" t="s">
@@ -16772,7 +16772,7 @@
         <v>1835</v>
       </c>
       <c r="AV12" s="84" t="s">
-        <v>2176</v>
+        <v>2169</v>
       </c>
     </row>
     <row r="13" spans="2:48">
@@ -16783,7 +16783,7 @@
         <v>1836</v>
       </c>
       <c r="D13" s="84" t="s">
-        <v>2354</v>
+        <v>2336</v>
       </c>
       <c r="E13" s="72"/>
       <c r="F13" s="82" t="s">
@@ -16793,7 +16793,7 @@
         <v>1836</v>
       </c>
       <c r="H13" s="84" t="s">
-        <v>1891</v>
+        <v>1890</v>
       </c>
       <c r="I13" s="72"/>
       <c r="J13" s="85"/>
@@ -16807,7 +16807,7 @@
         <v>1836</v>
       </c>
       <c r="P13" s="84" t="s">
-        <v>2085</v>
+        <v>2080</v>
       </c>
       <c r="Q13" s="72"/>
       <c r="R13" s="82" t="s">
@@ -16817,7 +16817,7 @@
         <v>1836</v>
       </c>
       <c r="T13" s="84" t="s">
-        <v>2172</v>
+        <v>2165</v>
       </c>
       <c r="U13" s="72"/>
       <c r="V13" s="82" t="s">
@@ -16827,7 +16827,7 @@
         <v>1836</v>
       </c>
       <c r="X13" s="84" t="s">
-        <v>2097</v>
+        <v>2091</v>
       </c>
       <c r="Y13" s="72"/>
       <c r="Z13" s="82" t="s">
@@ -16837,7 +16837,7 @@
         <v>1836</v>
       </c>
       <c r="AB13" s="84" t="s">
-        <v>2384</v>
+        <v>2363</v>
       </c>
       <c r="AC13" s="72"/>
       <c r="AD13" s="82" t="s">
@@ -16847,7 +16847,7 @@
         <v>1836</v>
       </c>
       <c r="AF13" s="84" t="s">
-        <v>2014</v>
+        <v>2011</v>
       </c>
       <c r="AG13" s="72"/>
       <c r="AH13" s="82" t="s">
@@ -16857,7 +16857,7 @@
         <v>1836</v>
       </c>
       <c r="AJ13" s="84" t="s">
-        <v>1894</v>
+        <v>1893</v>
       </c>
       <c r="AK13" s="72"/>
       <c r="AL13" s="82" t="s">
@@ -16867,7 +16867,7 @@
         <v>1836</v>
       </c>
       <c r="AN13" s="84" t="s">
-        <v>1895</v>
+        <v>1894</v>
       </c>
       <c r="AO13" s="72"/>
       <c r="AP13" s="82"/>
@@ -16881,7 +16881,7 @@
         <v>1836</v>
       </c>
       <c r="AV13" s="81" t="s">
-        <v>1896</v>
+        <v>1895</v>
       </c>
     </row>
     <row r="14" spans="2:48">
@@ -16892,7 +16892,7 @@
         <v>1837</v>
       </c>
       <c r="D14" s="84" t="s">
-        <v>2076</v>
+        <v>2072</v>
       </c>
       <c r="E14" s="72"/>
       <c r="F14" s="82" t="s">
@@ -16902,7 +16902,7 @@
         <v>1837</v>
       </c>
       <c r="H14" s="84" t="s">
-        <v>2362</v>
+        <v>2377</v>
       </c>
       <c r="I14" s="72"/>
       <c r="J14" s="85"/>
@@ -16916,7 +16916,7 @@
         <v>1837</v>
       </c>
       <c r="P14" s="84" t="s">
-        <v>1897</v>
+        <v>1896</v>
       </c>
       <c r="Q14" s="72"/>
       <c r="R14" s="82" t="s">
@@ -16926,7 +16926,7 @@
         <v>1837</v>
       </c>
       <c r="T14" s="84" t="s">
-        <v>2089</v>
+        <v>2368</v>
       </c>
       <c r="U14" s="72"/>
       <c r="V14" s="82" t="s">
@@ -16936,7 +16936,7 @@
         <v>1837</v>
       </c>
       <c r="X14" s="84" t="s">
-        <v>1898</v>
+        <v>1897</v>
       </c>
       <c r="Y14" s="72"/>
       <c r="Z14" s="82" t="s">
@@ -16946,7 +16946,7 @@
         <v>1837</v>
       </c>
       <c r="AB14" s="84" t="s">
-        <v>2145</v>
+        <v>2139</v>
       </c>
       <c r="AC14" s="72"/>
       <c r="AD14" s="82" t="s">
@@ -16956,7 +16956,7 @@
         <v>1837</v>
       </c>
       <c r="AF14" s="84" t="s">
-        <v>2272</v>
+        <v>2259</v>
       </c>
       <c r="AG14" s="72"/>
       <c r="AH14" s="82" t="s">
@@ -16966,7 +16966,7 @@
         <v>1837</v>
       </c>
       <c r="AJ14" s="84" t="s">
-        <v>2127</v>
+        <v>2121</v>
       </c>
       <c r="AK14" s="72"/>
       <c r="AL14" s="82" t="s">
@@ -16976,7 +16976,7 @@
         <v>1837</v>
       </c>
       <c r="AN14" s="84" t="s">
-        <v>1900</v>
+        <v>1899</v>
       </c>
       <c r="AO14" s="72"/>
       <c r="AP14" s="79" t="s">
@@ -16986,7 +16986,7 @@
         <v>1837</v>
       </c>
       <c r="AR14" s="81" t="s">
-        <v>2033</v>
+        <v>2029</v>
       </c>
       <c r="AS14" s="72"/>
       <c r="AT14" s="82"/>
@@ -17001,7 +17001,7 @@
         <v>1838</v>
       </c>
       <c r="D15" s="84" t="s">
-        <v>1901</v>
+        <v>1900</v>
       </c>
       <c r="E15" s="72"/>
       <c r="F15" s="85"/>
@@ -17019,7 +17019,7 @@
         <v>1838</v>
       </c>
       <c r="P15" s="84" t="s">
-        <v>1902</v>
+        <v>1901</v>
       </c>
       <c r="Q15" s="72"/>
       <c r="R15" s="82" t="s">
@@ -17029,7 +17029,7 @@
         <v>1838</v>
       </c>
       <c r="T15" s="84" t="s">
-        <v>2044</v>
+        <v>2040</v>
       </c>
       <c r="U15" s="72"/>
       <c r="V15" s="82" t="s">
@@ -17039,7 +17039,7 @@
         <v>1838</v>
       </c>
       <c r="X15" s="84" t="s">
-        <v>2092</v>
+        <v>2086</v>
       </c>
       <c r="Y15" s="72"/>
       <c r="Z15" s="82" t="s">
@@ -17049,7 +17049,7 @@
         <v>1838</v>
       </c>
       <c r="AB15" s="84" t="s">
-        <v>1903</v>
+        <v>1902</v>
       </c>
       <c r="AC15" s="72"/>
       <c r="AD15" s="82" t="s">
@@ -17059,7 +17059,7 @@
         <v>1838</v>
       </c>
       <c r="AF15" s="84" t="s">
-        <v>2111</v>
+        <v>2105</v>
       </c>
       <c r="AG15" s="72"/>
       <c r="AH15" s="85"/>
@@ -17073,7 +17073,7 @@
         <v>1838</v>
       </c>
       <c r="AN15" s="84" t="s">
-        <v>1904</v>
+        <v>1903</v>
       </c>
       <c r="AO15" s="72"/>
       <c r="AP15" s="82" t="s">
@@ -17083,7 +17083,7 @@
         <v>1838</v>
       </c>
       <c r="AR15" s="84" t="s">
-        <v>2140</v>
+        <v>2134</v>
       </c>
       <c r="AS15" s="72"/>
       <c r="AT15" s="82" t="s">
@@ -17093,7 +17093,7 @@
         <v>1838</v>
       </c>
       <c r="AV15" s="84" t="s">
-        <v>2149</v>
+        <v>2143</v>
       </c>
     </row>
     <row r="16" spans="2:48">
@@ -17104,7 +17104,7 @@
         <v>1839</v>
       </c>
       <c r="D16" s="84" t="s">
-        <v>2013</v>
+        <v>2010</v>
       </c>
       <c r="E16" s="72"/>
       <c r="F16" s="82" t="s">
@@ -17114,7 +17114,7 @@
         <v>1839</v>
       </c>
       <c r="H16" s="84" t="s">
-        <v>2374</v>
+        <v>2354</v>
       </c>
       <c r="I16" s="72"/>
       <c r="J16" s="85"/>
@@ -17128,7 +17128,7 @@
         <v>1839</v>
       </c>
       <c r="P16" s="84" t="s">
-        <v>1905</v>
+        <v>1904</v>
       </c>
       <c r="Q16" s="72"/>
       <c r="R16" s="82" t="s">
@@ -17138,7 +17138,7 @@
         <v>1839</v>
       </c>
       <c r="T16" s="84" t="s">
-        <v>2171</v>
+        <v>2164</v>
       </c>
       <c r="U16" s="72"/>
       <c r="V16" s="82" t="s">
@@ -17148,7 +17148,7 @@
         <v>1839</v>
       </c>
       <c r="X16" s="84" t="s">
-        <v>2091</v>
+        <v>2085</v>
       </c>
       <c r="Y16" s="72"/>
       <c r="Z16" s="82" t="s">
@@ -17158,7 +17158,7 @@
         <v>1839</v>
       </c>
       <c r="AB16" s="84" t="s">
-        <v>1907</v>
+        <v>1906</v>
       </c>
       <c r="AC16" s="72"/>
       <c r="AD16" s="82" t="s">
@@ -17168,7 +17168,7 @@
         <v>1839</v>
       </c>
       <c r="AF16" s="84" t="s">
-        <v>1908</v>
+        <v>1907</v>
       </c>
       <c r="AG16" s="72"/>
       <c r="AH16" s="82" t="s">
@@ -17178,7 +17178,7 @@
         <v>1839</v>
       </c>
       <c r="AJ16" s="84" t="s">
-        <v>2128</v>
+        <v>2122</v>
       </c>
       <c r="AK16" s="72"/>
       <c r="AL16" s="82" t="s">
@@ -17188,7 +17188,7 @@
         <v>1839</v>
       </c>
       <c r="AN16" s="84" t="s">
-        <v>2026</v>
+        <v>2022</v>
       </c>
       <c r="AO16" s="72"/>
       <c r="AP16" s="82" t="s">
@@ -17198,7 +17198,7 @@
         <v>1839</v>
       </c>
       <c r="AR16" s="84" t="s">
-        <v>2134</v>
+        <v>2128</v>
       </c>
       <c r="AS16" s="72"/>
       <c r="AT16" s="82" t="s">
@@ -17208,7 +17208,7 @@
         <v>1839</v>
       </c>
       <c r="AV16" s="84" t="s">
-        <v>2048</v>
+        <v>2044</v>
       </c>
     </row>
     <row r="17" spans="2:49">
@@ -17219,7 +17219,7 @@
         <v>1840</v>
       </c>
       <c r="D17" s="84" t="s">
-        <v>2041</v>
+        <v>2037</v>
       </c>
       <c r="E17" s="72"/>
       <c r="F17" s="82" t="s">
@@ -17229,7 +17229,7 @@
         <v>1840</v>
       </c>
       <c r="H17" s="84" t="s">
-        <v>2363</v>
+        <v>2343</v>
       </c>
       <c r="I17" s="72"/>
       <c r="J17" s="85"/>
@@ -17243,7 +17243,7 @@
         <v>1840</v>
       </c>
       <c r="P17" s="84" t="s">
-        <v>2124</v>
+        <v>2118</v>
       </c>
       <c r="Q17" s="72"/>
       <c r="R17" s="82" t="s">
@@ -17253,7 +17253,7 @@
         <v>1840</v>
       </c>
       <c r="T17" s="84" t="s">
-        <v>1909</v>
+        <v>1908</v>
       </c>
       <c r="U17" s="72"/>
       <c r="V17" s="82" t="s">
@@ -17263,7 +17263,7 @@
         <v>1840</v>
       </c>
       <c r="X17" s="84" t="s">
-        <v>2098</v>
+        <v>2092</v>
       </c>
       <c r="Y17" s="72"/>
       <c r="Z17" s="82" t="s">
@@ -17273,7 +17273,7 @@
         <v>1840</v>
       </c>
       <c r="AB17" s="84" t="s">
-        <v>2105</v>
+        <v>2099</v>
       </c>
       <c r="AC17" s="72"/>
       <c r="AD17" s="82" t="s">
@@ -17283,7 +17283,7 @@
         <v>1840</v>
       </c>
       <c r="AF17" s="84" t="s">
-        <v>1910</v>
+        <v>1909</v>
       </c>
       <c r="AG17" s="72"/>
       <c r="AH17" s="82" t="s">
@@ -17293,7 +17293,7 @@
         <v>1840</v>
       </c>
       <c r="AJ17" s="84" t="s">
-        <v>2170</v>
+        <v>2163</v>
       </c>
       <c r="AK17" s="72"/>
       <c r="AL17" s="82" t="s">
@@ -17303,7 +17303,7 @@
         <v>1840</v>
       </c>
       <c r="AN17" s="84" t="s">
-        <v>1911</v>
+        <v>1910</v>
       </c>
       <c r="AO17" s="72"/>
       <c r="AP17" s="82" t="s">
@@ -17313,7 +17313,7 @@
         <v>1840</v>
       </c>
       <c r="AR17" s="84" t="s">
-        <v>2136</v>
+        <v>2130</v>
       </c>
       <c r="AS17" s="72"/>
       <c r="AT17" s="82" t="s">
@@ -17323,7 +17323,7 @@
         <v>1840</v>
       </c>
       <c r="AV17" s="84" t="s">
-        <v>1912</v>
+        <v>1911</v>
       </c>
     </row>
     <row r="18" spans="2:49">
@@ -17334,7 +17334,7 @@
         <v>1841</v>
       </c>
       <c r="D18" s="84" t="s">
-        <v>2361</v>
+        <v>2342</v>
       </c>
       <c r="E18" s="72"/>
       <c r="F18" s="82" t="s">
@@ -17344,7 +17344,7 @@
         <v>1841</v>
       </c>
       <c r="H18" s="84" t="s">
-        <v>2230</v>
+        <v>2219</v>
       </c>
       <c r="I18" s="72"/>
       <c r="J18" s="85"/>
@@ -17358,7 +17358,7 @@
         <v>1841</v>
       </c>
       <c r="P18" s="84" t="s">
-        <v>2173</v>
+        <v>2166</v>
       </c>
       <c r="Q18" s="72"/>
       <c r="R18" s="82" t="s">
@@ -17368,7 +17368,7 @@
         <v>1841</v>
       </c>
       <c r="T18" s="84" t="s">
-        <v>2090</v>
+        <v>2084</v>
       </c>
       <c r="U18" s="72"/>
       <c r="V18" s="82" t="s">
@@ -17388,7 +17388,7 @@
         <v>1841</v>
       </c>
       <c r="AB18" s="84" t="s">
-        <v>1913</v>
+        <v>1912</v>
       </c>
       <c r="AC18" s="72"/>
       <c r="AD18" s="82" t="s">
@@ -17398,7 +17398,7 @@
         <v>1841</v>
       </c>
       <c r="AF18" s="84" t="s">
-        <v>2109</v>
+        <v>2103</v>
       </c>
       <c r="AG18" s="72"/>
       <c r="AH18" s="82" t="s">
@@ -17408,7 +17408,7 @@
         <v>1841</v>
       </c>
       <c r="AJ18" s="84" t="s">
-        <v>1914</v>
+        <v>1913</v>
       </c>
       <c r="AK18" s="72"/>
       <c r="AL18" s="85"/>
@@ -17422,7 +17422,7 @@
         <v>1841</v>
       </c>
       <c r="AR18" s="84" t="s">
-        <v>2307</v>
+        <v>2292</v>
       </c>
       <c r="AS18" s="72"/>
       <c r="AT18" s="82" t="s">
@@ -17432,7 +17432,7 @@
         <v>1841</v>
       </c>
       <c r="AV18" s="84" t="s">
-        <v>2049</v>
+        <v>2045</v>
       </c>
     </row>
     <row r="19" spans="2:49">
@@ -17443,7 +17443,7 @@
         <v>1842</v>
       </c>
       <c r="D19" s="84" t="s">
-        <v>2077</v>
+        <v>2073</v>
       </c>
       <c r="E19" s="72"/>
       <c r="F19" s="82" t="s">
@@ -17453,7 +17453,7 @@
         <v>1842</v>
       </c>
       <c r="H19" s="84" t="s">
-        <v>1915</v>
+        <v>1914</v>
       </c>
       <c r="I19" s="72"/>
       <c r="J19" s="85"/>
@@ -17467,7 +17467,7 @@
         <v>1842</v>
       </c>
       <c r="P19" s="84" t="s">
-        <v>1892</v>
+        <v>1891</v>
       </c>
       <c r="Q19" s="72"/>
       <c r="R19" s="82" t="s">
@@ -17477,7 +17477,7 @@
         <v>1842</v>
       </c>
       <c r="T19" s="84" t="s">
-        <v>1916</v>
+        <v>1915</v>
       </c>
       <c r="U19" s="72"/>
       <c r="V19" s="82" t="s">
@@ -17487,7 +17487,7 @@
         <v>1842</v>
       </c>
       <c r="X19" s="84" t="s">
-        <v>2174</v>
+        <v>2167</v>
       </c>
       <c r="Y19" s="72"/>
       <c r="Z19" s="82" t="s">
@@ -17497,7 +17497,7 @@
         <v>1842</v>
       </c>
       <c r="AB19" s="84" t="s">
-        <v>2198</v>
+        <v>2189</v>
       </c>
       <c r="AC19" s="72"/>
       <c r="AD19" s="82" t="s">
@@ -17507,7 +17507,7 @@
         <v>1842</v>
       </c>
       <c r="AF19" s="84" t="s">
-        <v>1893</v>
+        <v>1892</v>
       </c>
       <c r="AG19" s="72"/>
       <c r="AH19" s="82" t="s">
@@ -17517,7 +17517,7 @@
         <v>1842</v>
       </c>
       <c r="AJ19" s="84" t="s">
-        <v>2351</v>
+        <v>2333</v>
       </c>
       <c r="AK19" s="72"/>
       <c r="AL19" s="82" t="s">
@@ -17527,7 +17527,7 @@
         <v>1842</v>
       </c>
       <c r="AN19" s="84" t="s">
-        <v>1917</v>
+        <v>1916</v>
       </c>
       <c r="AO19" s="72"/>
       <c r="AP19" s="82" t="s">
@@ -17537,7 +17537,7 @@
         <v>1842</v>
       </c>
       <c r="AR19" s="84" t="s">
-        <v>1918</v>
+        <v>1917</v>
       </c>
       <c r="AS19" s="72"/>
       <c r="AT19" s="82" t="s">
@@ -17547,7 +17547,7 @@
         <v>1842</v>
       </c>
       <c r="AV19" s="84" t="s">
-        <v>2150</v>
+        <v>2144</v>
       </c>
     </row>
     <row r="20" spans="2:49">
@@ -17558,7 +17558,7 @@
         <v>1843</v>
       </c>
       <c r="D20" s="84" t="s">
-        <v>1919</v>
+        <v>1918</v>
       </c>
       <c r="E20" s="72"/>
       <c r="F20" s="82" t="s">
@@ -17568,7 +17568,7 @@
         <v>1843</v>
       </c>
       <c r="H20" s="84" t="s">
-        <v>2043</v>
+        <v>2039</v>
       </c>
       <c r="I20" s="72"/>
       <c r="J20" s="85"/>
@@ -17582,7 +17582,7 @@
         <v>1843</v>
       </c>
       <c r="P20" s="84" t="s">
-        <v>2119</v>
+        <v>2113</v>
       </c>
       <c r="Q20" s="72"/>
       <c r="R20" s="82" t="s">
@@ -17592,7 +17592,7 @@
         <v>1843</v>
       </c>
       <c r="T20" s="84" t="s">
-        <v>2157</v>
+        <v>2151</v>
       </c>
       <c r="U20" s="72"/>
       <c r="V20" s="82" t="s">
@@ -17602,7 +17602,7 @@
         <v>1843</v>
       </c>
       <c r="X20" s="84" t="s">
-        <v>2093</v>
+        <v>2087</v>
       </c>
       <c r="Y20" s="72"/>
       <c r="Z20" s="82" t="s">
@@ -17612,7 +17612,7 @@
         <v>1843</v>
       </c>
       <c r="AB20" s="84" t="s">
-        <v>2197</v>
+        <v>2188</v>
       </c>
       <c r="AC20" s="72"/>
       <c r="AD20" s="82" t="s">
@@ -17622,7 +17622,7 @@
         <v>1843</v>
       </c>
       <c r="AF20" s="84" t="s">
-        <v>2240</v>
+        <v>2229</v>
       </c>
       <c r="AG20" s="72"/>
       <c r="AH20" s="82" t="s">
@@ -17632,7 +17632,7 @@
         <v>1843</v>
       </c>
       <c r="AJ20" s="84" t="s">
-        <v>2352</v>
+        <v>2334</v>
       </c>
       <c r="AK20" s="72"/>
       <c r="AL20" s="82" t="s">
@@ -17642,7 +17642,7 @@
         <v>1843</v>
       </c>
       <c r="AN20" s="84" t="s">
-        <v>1920</v>
+        <v>1919</v>
       </c>
       <c r="AO20" s="72"/>
       <c r="AP20" s="82" t="s">
@@ -17652,7 +17652,7 @@
         <v>1843</v>
       </c>
       <c r="AR20" s="84" t="s">
-        <v>2137</v>
+        <v>2131</v>
       </c>
       <c r="AS20" s="72"/>
       <c r="AT20" s="82" t="s">
@@ -17662,7 +17662,7 @@
         <v>1843</v>
       </c>
       <c r="AV20" s="84" t="s">
-        <v>2151</v>
+        <v>2145</v>
       </c>
     </row>
     <row r="21" spans="2:49">
@@ -17673,7 +17673,7 @@
         <v>1844</v>
       </c>
       <c r="D21" s="84" t="s">
-        <v>2078</v>
+        <v>2074</v>
       </c>
       <c r="E21" s="72"/>
       <c r="F21" s="82" t="s">
@@ -17683,7 +17683,7 @@
         <v>1844</v>
       </c>
       <c r="H21" s="84" t="s">
-        <v>1921</v>
+        <v>1920</v>
       </c>
       <c r="I21" s="72"/>
       <c r="J21" s="85"/>
@@ -17697,7 +17697,7 @@
         <v>1844</v>
       </c>
       <c r="P21" s="84" t="s">
-        <v>2120</v>
+        <v>2114</v>
       </c>
       <c r="Q21" s="72"/>
       <c r="R21" s="82" t="s">
@@ -17707,7 +17707,7 @@
         <v>1844</v>
       </c>
       <c r="T21" s="84" t="s">
-        <v>2117</v>
+        <v>2111</v>
       </c>
       <c r="U21" s="72"/>
       <c r="V21" s="82" t="s">
@@ -17717,7 +17717,7 @@
         <v>1844</v>
       </c>
       <c r="X21" s="84" t="s">
-        <v>2094</v>
+        <v>2088</v>
       </c>
       <c r="Y21" s="72"/>
       <c r="Z21" s="82" t="s">
@@ -17727,7 +17727,7 @@
         <v>1844</v>
       </c>
       <c r="AB21" s="84" t="s">
-        <v>2102</v>
+        <v>2096</v>
       </c>
       <c r="AC21" s="72"/>
       <c r="AD21" s="82" t="s">
@@ -17737,7 +17737,7 @@
         <v>1844</v>
       </c>
       <c r="AF21" s="84" t="s">
-        <v>2114</v>
+        <v>2108</v>
       </c>
       <c r="AG21" s="72"/>
       <c r="AH21" s="82" t="s">
@@ -17747,7 +17747,7 @@
         <v>1844</v>
       </c>
       <c r="AJ21" s="84" t="s">
-        <v>2130</v>
+        <v>2124</v>
       </c>
       <c r="AK21" s="72"/>
       <c r="AL21" s="82" t="s">
@@ -17757,7 +17757,7 @@
         <v>1844</v>
       </c>
       <c r="AN21" s="84" t="s">
-        <v>2324</v>
+        <v>2309</v>
       </c>
       <c r="AO21" s="72"/>
       <c r="AP21" s="82" t="s">
@@ -17767,7 +17767,7 @@
         <v>1844</v>
       </c>
       <c r="AR21" s="84" t="s">
-        <v>1922</v>
+        <v>1921</v>
       </c>
       <c r="AS21" s="72"/>
       <c r="AT21" s="82" t="s">
@@ -17777,7 +17777,7 @@
         <v>1844</v>
       </c>
       <c r="AV21" s="84" t="s">
-        <v>2152</v>
+        <v>2146</v>
       </c>
     </row>
     <row r="22" spans="2:49">
@@ -17788,7 +17788,7 @@
         <v>1845</v>
       </c>
       <c r="D22" s="84" t="s">
-        <v>2333</v>
+        <v>2317</v>
       </c>
       <c r="E22" s="72"/>
       <c r="F22" s="82" t="s">
@@ -17798,7 +17798,7 @@
         <v>1845</v>
       </c>
       <c r="H22" s="84" t="s">
-        <v>2143</v>
+        <v>2137</v>
       </c>
       <c r="I22" s="72"/>
       <c r="J22" s="85"/>
@@ -17812,7 +17812,7 @@
         <v>1845</v>
       </c>
       <c r="P22" s="84" t="s">
-        <v>2086</v>
+        <v>2081</v>
       </c>
       <c r="Q22" s="72"/>
       <c r="R22" s="82" t="s">
@@ -17822,7 +17822,7 @@
         <v>1845</v>
       </c>
       <c r="T22" s="84" t="s">
-        <v>2365</v>
+        <v>2345</v>
       </c>
       <c r="U22" s="72"/>
       <c r="V22" s="82" t="s">
@@ -17832,7 +17832,7 @@
         <v>1845</v>
       </c>
       <c r="X22" s="84" t="s">
-        <v>2364</v>
+        <v>2344</v>
       </c>
       <c r="Y22" s="72"/>
       <c r="Z22" s="82" t="s">
@@ -17842,7 +17842,7 @@
         <v>1845</v>
       </c>
       <c r="AB22" s="84" t="s">
-        <v>2212</v>
+        <v>2202</v>
       </c>
       <c r="AC22" s="72"/>
       <c r="AD22" s="82" t="s">
@@ -17852,7 +17852,7 @@
         <v>1845</v>
       </c>
       <c r="AF22" s="84" t="s">
-        <v>2106</v>
+        <v>2100</v>
       </c>
       <c r="AG22" s="72"/>
       <c r="AH22" s="82" t="s">
@@ -17862,7 +17862,7 @@
         <v>1845</v>
       </c>
       <c r="AJ22" s="84" t="s">
-        <v>2327</v>
+        <v>2312</v>
       </c>
       <c r="AK22" s="72"/>
       <c r="AL22" s="82" t="s">
@@ -17872,7 +17872,7 @@
         <v>1845</v>
       </c>
       <c r="AN22" s="84" t="s">
-        <v>1923</v>
+        <v>1922</v>
       </c>
       <c r="AO22" s="72"/>
       <c r="AP22" s="82" t="s">
@@ -17882,7 +17882,7 @@
         <v>1845</v>
       </c>
       <c r="AR22" s="84" t="s">
-        <v>2138</v>
+        <v>2132</v>
       </c>
       <c r="AS22" s="72"/>
       <c r="AT22" s="82" t="s">
@@ -17892,7 +17892,7 @@
         <v>1845</v>
       </c>
       <c r="AV22" s="84" t="s">
-        <v>2153</v>
+        <v>2147</v>
       </c>
     </row>
     <row r="23" spans="2:49">
@@ -17903,7 +17903,7 @@
         <v>1846</v>
       </c>
       <c r="D23" s="84" t="s">
-        <v>2042</v>
+        <v>2038</v>
       </c>
       <c r="E23" s="72"/>
       <c r="F23" s="82" t="s">
@@ -17913,7 +17913,7 @@
         <v>1846</v>
       </c>
       <c r="H23" s="84" t="s">
-        <v>1924</v>
+        <v>1923</v>
       </c>
       <c r="I23" s="72"/>
       <c r="J23" s="85"/>
@@ -17927,7 +17927,7 @@
         <v>1846</v>
       </c>
       <c r="P23" s="84" t="s">
-        <v>2274</v>
+        <v>2261</v>
       </c>
       <c r="Q23" s="72"/>
       <c r="R23" s="82" t="s">
@@ -17937,7 +17937,7 @@
         <v>1846</v>
       </c>
       <c r="T23" s="84" t="s">
-        <v>2357</v>
+        <v>2339</v>
       </c>
       <c r="U23" s="72"/>
       <c r="V23" s="82" t="s">
@@ -17947,7 +17947,7 @@
         <v>1846</v>
       </c>
       <c r="X23" s="84" t="s">
-        <v>2279</v>
+        <v>2266</v>
       </c>
       <c r="Y23" s="72"/>
       <c r="Z23" s="82" t="s">
@@ -17957,7 +17957,7 @@
         <v>1846</v>
       </c>
       <c r="AB23" s="84" t="s">
-        <v>2103</v>
+        <v>2097</v>
       </c>
       <c r="AC23" s="72"/>
       <c r="AD23" s="82" t="s">
@@ -17967,7 +17967,7 @@
         <v>1846</v>
       </c>
       <c r="AF23" s="84" t="s">
-        <v>2241</v>
+        <v>2230</v>
       </c>
       <c r="AG23" s="72"/>
       <c r="AH23" s="82" t="s">
@@ -17977,7 +17977,7 @@
         <v>1846</v>
       </c>
       <c r="AJ23" s="84" t="s">
-        <v>2310</v>
+        <v>2295</v>
       </c>
       <c r="AK23" s="72"/>
       <c r="AL23" s="82" t="s">
@@ -17987,7 +17987,7 @@
         <v>1846</v>
       </c>
       <c r="AN23" s="84" t="s">
-        <v>2133</v>
+        <v>2127</v>
       </c>
       <c r="AO23" s="72"/>
       <c r="AP23" s="82" t="s">
@@ -17997,7 +17997,7 @@
         <v>1846</v>
       </c>
       <c r="AR23" s="84" t="s">
-        <v>2139</v>
+        <v>2133</v>
       </c>
       <c r="AS23" s="72"/>
       <c r="AT23" s="82" t="s">
@@ -18018,7 +18018,7 @@
         <v>1847</v>
       </c>
       <c r="D24" s="84" t="s">
-        <v>2368</v>
+        <v>2348</v>
       </c>
       <c r="E24" s="72"/>
       <c r="F24" s="82" t="s">
@@ -18028,7 +18028,7 @@
         <v>1847</v>
       </c>
       <c r="H24" s="84" t="s">
-        <v>1925</v>
+        <v>1924</v>
       </c>
       <c r="I24" s="72"/>
       <c r="J24" s="85"/>
@@ -18042,7 +18042,7 @@
         <v>1847</v>
       </c>
       <c r="P24" s="84" t="s">
-        <v>2118</v>
+        <v>2112</v>
       </c>
       <c r="Q24" s="72"/>
       <c r="R24" s="82" t="s">
@@ -18052,7 +18052,7 @@
         <v>1847</v>
       </c>
       <c r="T24" s="84" t="s">
-        <v>1926</v>
+        <v>1925</v>
       </c>
       <c r="U24" s="72"/>
       <c r="V24" s="82" t="s">
@@ -18062,7 +18062,7 @@
         <v>1847</v>
       </c>
       <c r="X24" s="84" t="s">
-        <v>1927</v>
+        <v>1926</v>
       </c>
       <c r="Y24" s="72"/>
       <c r="Z24" s="82" t="s">
@@ -18072,7 +18072,7 @@
         <v>1847</v>
       </c>
       <c r="AB24" s="84" t="s">
-        <v>2329</v>
+        <v>2314</v>
       </c>
       <c r="AC24" s="72"/>
       <c r="AD24" s="82" t="s">
@@ -18082,7 +18082,7 @@
         <v>1847</v>
       </c>
       <c r="AF24" s="84" t="s">
-        <v>2359</v>
+        <v>2340</v>
       </c>
       <c r="AG24" s="72"/>
       <c r="AH24" s="82" t="s">
@@ -18092,7 +18092,7 @@
         <v>1847</v>
       </c>
       <c r="AJ24" s="84" t="s">
-        <v>2325</v>
+        <v>2310</v>
       </c>
       <c r="AK24" s="72"/>
       <c r="AL24" s="82" t="s">
@@ -18102,7 +18102,7 @@
         <v>1847</v>
       </c>
       <c r="AN24" s="84" t="s">
-        <v>1928</v>
+        <v>1927</v>
       </c>
       <c r="AO24" s="72"/>
       <c r="AP24" s="82" t="s">
@@ -18112,7 +18112,7 @@
         <v>1847</v>
       </c>
       <c r="AR24" s="84" t="s">
-        <v>2141</v>
+        <v>2135</v>
       </c>
       <c r="AS24" s="72"/>
       <c r="AT24" s="82" t="s">
@@ -18122,7 +18122,7 @@
         <v>1847</v>
       </c>
       <c r="AV24" s="84" t="s">
-        <v>2322</v>
+        <v>2307</v>
       </c>
     </row>
     <row r="25" spans="2:49">
@@ -18133,7 +18133,7 @@
         <v>1848</v>
       </c>
       <c r="D25" s="84" t="s">
-        <v>2355</v>
+        <v>2337</v>
       </c>
       <c r="E25" s="72"/>
       <c r="F25" s="82" t="s">
@@ -18143,7 +18143,7 @@
         <v>1848</v>
       </c>
       <c r="H25" s="84" t="s">
-        <v>1929</v>
+        <v>1928</v>
       </c>
       <c r="I25" s="72"/>
       <c r="J25" s="85"/>
@@ -18157,7 +18157,7 @@
         <v>1848</v>
       </c>
       <c r="P25" s="84" t="s">
-        <v>2123</v>
+        <v>2117</v>
       </c>
       <c r="Q25" s="72"/>
       <c r="R25" s="82" t="s">
@@ -18167,7 +18167,7 @@
         <v>1848</v>
       </c>
       <c r="T25" s="84" t="s">
-        <v>2326</v>
+        <v>2311</v>
       </c>
       <c r="U25" s="72"/>
       <c r="V25" s="82" t="s">
@@ -18177,7 +18177,7 @@
         <v>1848</v>
       </c>
       <c r="X25" s="84" t="s">
-        <v>2366</v>
+        <v>2346</v>
       </c>
       <c r="Y25" s="72"/>
       <c r="Z25" s="82" t="s">
@@ -18187,7 +18187,7 @@
         <v>1848</v>
       </c>
       <c r="AB25" s="84" t="s">
-        <v>2024</v>
+        <v>2020</v>
       </c>
       <c r="AC25" s="72"/>
       <c r="AD25" s="82" t="s">
@@ -18197,7 +18197,7 @@
         <v>1848</v>
       </c>
       <c r="AF25" s="84" t="s">
-        <v>2112</v>
+        <v>2106</v>
       </c>
       <c r="AG25" s="72"/>
       <c r="AH25" s="82" t="s">
@@ -18207,7 +18207,7 @@
         <v>1848</v>
       </c>
       <c r="AJ25" s="84" t="s">
-        <v>2131</v>
+        <v>2125</v>
       </c>
       <c r="AK25" s="72"/>
       <c r="AL25" s="82" t="s">
@@ -18217,7 +18217,7 @@
         <v>1848</v>
       </c>
       <c r="AN25" s="84" t="s">
-        <v>2129</v>
+        <v>2123</v>
       </c>
       <c r="AO25" s="72"/>
       <c r="AP25" s="82" t="s">
@@ -18227,7 +18227,7 @@
         <v>1848</v>
       </c>
       <c r="AR25" s="84" t="s">
-        <v>2046</v>
+        <v>2042</v>
       </c>
       <c r="AS25" s="72"/>
       <c r="AT25" s="82" t="s">
@@ -18237,7 +18237,7 @@
         <v>1848</v>
       </c>
       <c r="AV25" s="84" t="s">
-        <v>2177</v>
+        <v>2170</v>
       </c>
     </row>
     <row r="26" spans="2:49" ht="15.75" thickBot="1">
@@ -18248,7 +18248,7 @@
         <v>1849</v>
       </c>
       <c r="D26" s="91" t="s">
-        <v>1930</v>
+        <v>1929</v>
       </c>
       <c r="E26" s="72"/>
       <c r="F26" s="89" t="s">
@@ -18258,7 +18258,7 @@
         <v>1849</v>
       </c>
       <c r="H26" s="91" t="s">
-        <v>1931</v>
+        <v>1930</v>
       </c>
       <c r="I26" s="72"/>
       <c r="J26" s="92"/>
@@ -18272,7 +18272,7 @@
         <v>1849</v>
       </c>
       <c r="P26" s="91" t="s">
-        <v>2087</v>
+        <v>2082</v>
       </c>
       <c r="Q26" s="72"/>
       <c r="R26" s="89" t="s">
@@ -18282,7 +18282,7 @@
         <v>1849</v>
       </c>
       <c r="T26" s="91" t="s">
-        <v>1932</v>
+        <v>1931</v>
       </c>
       <c r="U26" s="72"/>
       <c r="V26" s="89" t="s">
@@ -18292,7 +18292,7 @@
         <v>1849</v>
       </c>
       <c r="X26" s="91" t="s">
-        <v>2099</v>
+        <v>2093</v>
       </c>
       <c r="Y26" s="72"/>
       <c r="Z26" s="89" t="s">
@@ -18302,7 +18302,7 @@
         <v>1849</v>
       </c>
       <c r="AB26" s="91" t="s">
-        <v>2104</v>
+        <v>2098</v>
       </c>
       <c r="AC26" s="72"/>
       <c r="AD26" s="89" t="s">
@@ -18312,7 +18312,7 @@
         <v>1849</v>
       </c>
       <c r="AF26" s="91" t="s">
-        <v>2110</v>
+        <v>2104</v>
       </c>
       <c r="AG26" s="72"/>
       <c r="AH26" s="89" t="s">
@@ -18322,7 +18322,7 @@
         <v>1849</v>
       </c>
       <c r="AJ26" s="91" t="s">
-        <v>2331</v>
+        <v>2316</v>
       </c>
       <c r="AK26" s="72"/>
       <c r="AL26" s="89" t="s">
@@ -18332,7 +18332,7 @@
         <v>1849</v>
       </c>
       <c r="AN26" s="91" t="s">
-        <v>2113</v>
+        <v>2107</v>
       </c>
       <c r="AO26" s="72"/>
       <c r="AP26" s="89" t="s">
@@ -18342,7 +18342,7 @@
         <v>1849</v>
       </c>
       <c r="AR26" s="91" t="s">
-        <v>2047</v>
+        <v>2043</v>
       </c>
       <c r="AS26" s="72"/>
       <c r="AT26" s="89" t="s">
@@ -18352,7 +18352,7 @@
         <v>1849</v>
       </c>
       <c r="AV26" s="91" t="s">
-        <v>2155</v>
+        <v>2149</v>
       </c>
     </row>
     <row r="27" spans="2:49" ht="24" customHeight="1" thickBot="1">
@@ -18412,7 +18412,7 @@
         <v>1826</v>
       </c>
       <c r="D28" s="71" t="s">
-        <v>2168</v>
+        <v>2161</v>
       </c>
       <c r="E28" s="72"/>
       <c r="F28" s="69" t="s">
@@ -18422,7 +18422,7 @@
         <v>1826</v>
       </c>
       <c r="H28" s="71" t="s">
-        <v>2162</v>
+        <v>2155</v>
       </c>
       <c r="I28" s="72"/>
       <c r="J28" s="69" t="s">
@@ -18432,7 +18432,7 @@
         <v>1826</v>
       </c>
       <c r="L28" s="71" t="s">
-        <v>2050</v>
+        <v>2046</v>
       </c>
       <c r="M28" s="72"/>
       <c r="N28" s="69" t="s">
@@ -18442,7 +18442,7 @@
         <v>1826</v>
       </c>
       <c r="P28" s="71" t="s">
-        <v>2277</v>
+        <v>2264</v>
       </c>
       <c r="Q28" s="72"/>
       <c r="R28" s="69" t="s">
@@ -18452,7 +18452,7 @@
         <v>1826</v>
       </c>
       <c r="T28" s="71" t="s">
-        <v>2304</v>
+        <v>2290</v>
       </c>
       <c r="U28" s="72"/>
       <c r="V28" s="69" t="s">
@@ -18462,7 +18462,7 @@
         <v>1826</v>
       </c>
       <c r="X28" s="71" t="s">
-        <v>1933</v>
+        <v>1932</v>
       </c>
       <c r="Y28" s="72"/>
       <c r="Z28" s="69" t="s">
@@ -18472,7 +18472,7 @@
         <v>1826</v>
       </c>
       <c r="AB28" s="71" t="s">
-        <v>2214</v>
+        <v>2204</v>
       </c>
       <c r="AC28" s="72"/>
       <c r="AD28" s="69" t="s">
@@ -18482,7 +18482,7 @@
         <v>1826</v>
       </c>
       <c r="AF28" s="71" t="s">
-        <v>2242</v>
+        <v>2231</v>
       </c>
       <c r="AG28" s="72"/>
       <c r="AH28" s="69" t="s">
@@ -18492,7 +18492,7 @@
         <v>1826</v>
       </c>
       <c r="AJ28" s="71" t="s">
-        <v>2054</v>
+        <v>2050</v>
       </c>
       <c r="AK28" s="72"/>
       <c r="AL28" s="69" t="s">
@@ -18502,7 +18502,7 @@
         <v>1826</v>
       </c>
       <c r="AN28" s="71" t="s">
-        <v>2282</v>
+        <v>2269</v>
       </c>
       <c r="AO28" s="72"/>
       <c r="AP28" s="69" t="s">
@@ -18512,7 +18512,7 @@
         <v>1826</v>
       </c>
       <c r="AR28" s="71" t="s">
-        <v>2249</v>
+        <v>2382</v>
       </c>
       <c r="AS28" s="72"/>
       <c r="AT28" s="69" t="s">
@@ -18522,7 +18522,7 @@
         <v>1826</v>
       </c>
       <c r="AV28" s="71" t="s">
-        <v>2253</v>
+        <v>2242</v>
       </c>
       <c r="AW28" s="65"/>
     </row>
@@ -18538,7 +18538,7 @@
         <v>1827</v>
       </c>
       <c r="H29" s="84" t="s">
-        <v>2373</v>
+        <v>2353</v>
       </c>
       <c r="I29" s="72"/>
       <c r="J29" s="82" t="s">
@@ -18548,7 +18548,7 @@
         <v>1827</v>
       </c>
       <c r="L29" s="84" t="s">
-        <v>1934</v>
+        <v>1933</v>
       </c>
       <c r="M29" s="72"/>
       <c r="N29" s="82" t="s">
@@ -18558,7 +18558,7 @@
         <v>1827</v>
       </c>
       <c r="P29" s="84" t="s">
-        <v>2341</v>
+        <v>2324</v>
       </c>
       <c r="Q29" s="72"/>
       <c r="R29" s="82" t="s">
@@ -18568,7 +18568,7 @@
         <v>1827</v>
       </c>
       <c r="T29" s="84" t="s">
-        <v>1935</v>
+        <v>1934</v>
       </c>
       <c r="U29" s="72"/>
       <c r="V29" s="82" t="s">
@@ -18578,7 +18578,7 @@
         <v>1827</v>
       </c>
       <c r="X29" s="84" t="s">
-        <v>2203</v>
+        <v>2194</v>
       </c>
       <c r="Y29" s="72"/>
       <c r="Z29" s="82" t="s">
@@ -18588,7 +18588,7 @@
         <v>1827</v>
       </c>
       <c r="AB29" s="84" t="s">
-        <v>1936</v>
+        <v>1935</v>
       </c>
       <c r="AC29" s="72"/>
       <c r="AD29" s="82" t="s">
@@ -18598,7 +18598,7 @@
         <v>1827</v>
       </c>
       <c r="AF29" s="84" t="s">
-        <v>1937</v>
+        <v>1936</v>
       </c>
       <c r="AG29" s="72"/>
       <c r="AH29" s="82" t="s">
@@ -18608,7 +18608,7 @@
         <v>1827</v>
       </c>
       <c r="AJ29" s="84" t="s">
-        <v>2308</v>
+        <v>2293</v>
       </c>
       <c r="AK29" s="72"/>
       <c r="AL29" s="82" t="s">
@@ -18618,7 +18618,7 @@
         <v>1827</v>
       </c>
       <c r="AN29" s="84" t="s">
-        <v>2292</v>
+        <v>2278</v>
       </c>
       <c r="AO29" s="72"/>
       <c r="AP29" s="82" t="s">
@@ -18628,7 +18628,7 @@
         <v>1827</v>
       </c>
       <c r="AR29" s="84" t="s">
-        <v>1938</v>
+        <v>1937</v>
       </c>
       <c r="AS29" s="72"/>
       <c r="AT29" s="82" t="s">
@@ -18638,7 +18638,7 @@
         <v>1827</v>
       </c>
       <c r="AV29" s="84" t="s">
-        <v>2254</v>
+        <v>2243</v>
       </c>
       <c r="AW29" s="65"/>
     </row>
@@ -18700,7 +18700,7 @@
         <v>1829</v>
       </c>
       <c r="D31" s="84" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
       <c r="E31" s="72"/>
       <c r="F31" s="82" t="s">
@@ -18710,7 +18710,7 @@
         <v>1829</v>
       </c>
       <c r="H31" s="84" t="s">
-        <v>1981</v>
+        <v>1978</v>
       </c>
       <c r="I31" s="72"/>
       <c r="J31" s="82" t="s">
@@ -18720,7 +18720,7 @@
         <v>1829</v>
       </c>
       <c r="L31" s="84" t="s">
-        <v>1942</v>
+        <v>1941</v>
       </c>
       <c r="M31" s="72"/>
       <c r="N31" s="82" t="s">
@@ -18730,7 +18730,7 @@
         <v>1829</v>
       </c>
       <c r="P31" s="84" t="s">
-        <v>1943</v>
+        <v>1942</v>
       </c>
       <c r="Q31" s="72"/>
       <c r="R31" s="82" t="s">
@@ -18740,7 +18740,7 @@
         <v>1829</v>
       </c>
       <c r="T31" s="84" t="s">
-        <v>2305</v>
+        <v>2376</v>
       </c>
       <c r="U31" s="72"/>
       <c r="V31" s="82" t="s">
@@ -18750,7 +18750,7 @@
         <v>1829</v>
       </c>
       <c r="X31" s="84" t="s">
-        <v>2204</v>
+        <v>2195</v>
       </c>
       <c r="Y31" s="72"/>
       <c r="Z31" s="82" t="s">
@@ -18760,7 +18760,7 @@
         <v>1829</v>
       </c>
       <c r="AB31" s="84" t="s">
-        <v>2175</v>
+        <v>2168</v>
       </c>
       <c r="AC31" s="72"/>
       <c r="AD31" s="82" t="s">
@@ -18770,7 +18770,7 @@
         <v>1829</v>
       </c>
       <c r="AF31" s="84" t="s">
-        <v>2053</v>
+        <v>2049</v>
       </c>
       <c r="AG31" s="72"/>
       <c r="AH31" s="82" t="s">
@@ -18780,7 +18780,7 @@
         <v>1829</v>
       </c>
       <c r="AJ31" s="84" t="s">
-        <v>1944</v>
+        <v>1943</v>
       </c>
       <c r="AK31" s="72"/>
       <c r="AL31" s="82" t="s">
@@ -18790,7 +18790,7 @@
         <v>1829</v>
       </c>
       <c r="AN31" s="84" t="s">
-        <v>2293</v>
+        <v>2279</v>
       </c>
       <c r="AO31" s="72"/>
       <c r="AP31" s="82" t="s">
@@ -18800,7 +18800,7 @@
         <v>1829</v>
       </c>
       <c r="AR31" s="84" t="s">
-        <v>2250</v>
+        <v>2239</v>
       </c>
       <c r="AS31" s="72"/>
       <c r="AT31" s="82" t="s">
@@ -18810,7 +18810,7 @@
         <v>1829</v>
       </c>
       <c r="AV31" s="84" t="s">
-        <v>2255</v>
+        <v>2244</v>
       </c>
       <c r="AW31" s="65"/>
     </row>
@@ -18822,7 +18822,7 @@
         <v>1830</v>
       </c>
       <c r="D32" s="84" t="s">
-        <v>2356</v>
+        <v>2338</v>
       </c>
       <c r="E32" s="72"/>
       <c r="F32" s="82" t="s">
@@ -18832,7 +18832,7 @@
         <v>1830</v>
       </c>
       <c r="H32" s="84" t="s">
-        <v>2163</v>
+        <v>2156</v>
       </c>
       <c r="I32" s="72"/>
       <c r="J32" s="82" t="s">
@@ -18842,7 +18842,7 @@
         <v>1830</v>
       </c>
       <c r="L32" s="84" t="s">
-        <v>2051</v>
+        <v>2047</v>
       </c>
       <c r="M32" s="72"/>
       <c r="N32" s="82" t="s">
@@ -18852,7 +18852,7 @@
         <v>1830</v>
       </c>
       <c r="P32" s="84" t="s">
-        <v>2181</v>
+        <v>2174</v>
       </c>
       <c r="Q32" s="72"/>
       <c r="R32" s="82" t="s">
@@ -18862,7 +18862,7 @@
         <v>1830</v>
       </c>
       <c r="T32" s="84" t="s">
-        <v>2306</v>
+        <v>2291</v>
       </c>
       <c r="U32" s="72"/>
       <c r="V32" s="82" t="s">
@@ -18872,7 +18872,7 @@
         <v>1830</v>
       </c>
       <c r="X32" s="84" t="s">
-        <v>2347</v>
+        <v>2330</v>
       </c>
       <c r="Y32" s="72"/>
       <c r="Z32" s="82" t="s">
@@ -18882,7 +18882,7 @@
         <v>1830</v>
       </c>
       <c r="AB32" s="84" t="s">
-        <v>2225</v>
+        <v>2215</v>
       </c>
       <c r="AC32" s="72"/>
       <c r="AD32" s="82" t="s">
@@ -18892,7 +18892,7 @@
         <v>1830</v>
       </c>
       <c r="AF32" s="84" t="s">
-        <v>2231</v>
+        <v>2220</v>
       </c>
       <c r="AG32" s="72"/>
       <c r="AH32" s="82" t="s">
@@ -18902,7 +18902,7 @@
         <v>1830</v>
       </c>
       <c r="AJ32" s="84" t="s">
-        <v>2311</v>
+        <v>2296</v>
       </c>
       <c r="AK32" s="72"/>
       <c r="AL32" s="82" t="s">
@@ -18912,7 +18912,7 @@
         <v>1830</v>
       </c>
       <c r="AN32" s="84" t="s">
-        <v>2295</v>
+        <v>2281</v>
       </c>
       <c r="AO32" s="72"/>
       <c r="AP32" s="82" t="s">
@@ -18922,7 +18922,7 @@
         <v>1830</v>
       </c>
       <c r="AR32" s="84" t="s">
-        <v>2276</v>
+        <v>2263</v>
       </c>
       <c r="AS32" s="72"/>
       <c r="AT32" s="82" t="s">
@@ -18932,7 +18932,7 @@
         <v>1830</v>
       </c>
       <c r="AV32" s="84" t="s">
-        <v>2256</v>
+        <v>2245</v>
       </c>
       <c r="AW32" s="65"/>
     </row>
@@ -18944,7 +18944,7 @@
         <v>1831</v>
       </c>
       <c r="D33" s="84" t="s">
-        <v>1945</v>
+        <v>2366</v>
       </c>
       <c r="E33" s="72"/>
       <c r="F33" s="82" t="s">
@@ -18954,7 +18954,7 @@
         <v>1831</v>
       </c>
       <c r="H33" s="84" t="s">
-        <v>1946</v>
+        <v>1944</v>
       </c>
       <c r="I33" s="72"/>
       <c r="J33" s="82" t="s">
@@ -18964,7 +18964,7 @@
         <v>1831</v>
       </c>
       <c r="L33" s="84" t="s">
-        <v>2320</v>
+        <v>2305</v>
       </c>
       <c r="M33" s="72"/>
       <c r="N33" s="82" t="s">
@@ -18974,7 +18974,7 @@
         <v>1831</v>
       </c>
       <c r="P33" s="84" t="s">
-        <v>2052</v>
+        <v>2048</v>
       </c>
       <c r="Q33" s="72"/>
       <c r="R33" s="82" t="s">
@@ -18984,7 +18984,7 @@
         <v>1831</v>
       </c>
       <c r="T33" s="84" t="s">
-        <v>2199</v>
+        <v>2190</v>
       </c>
       <c r="U33" s="72"/>
       <c r="V33" s="82" t="s">
@@ -18994,7 +18994,7 @@
         <v>1831</v>
       </c>
       <c r="X33" s="84" t="s">
-        <v>2031</v>
+        <v>2027</v>
       </c>
       <c r="Y33" s="72"/>
       <c r="Z33" s="82" t="s">
@@ -19004,7 +19004,7 @@
         <v>1831</v>
       </c>
       <c r="AB33" s="84" t="s">
-        <v>2226</v>
+        <v>2216</v>
       </c>
       <c r="AC33" s="72"/>
       <c r="AD33" s="82" t="s">
@@ -19014,7 +19014,7 @@
         <v>1831</v>
       </c>
       <c r="AF33" s="84" t="s">
-        <v>2270</v>
+        <v>2257</v>
       </c>
       <c r="AG33" s="72"/>
       <c r="AH33" s="82" t="s">
@@ -19024,7 +19024,7 @@
         <v>1831</v>
       </c>
       <c r="AJ33" s="84" t="s">
-        <v>1948</v>
+        <v>1946</v>
       </c>
       <c r="AK33" s="72"/>
       <c r="AL33" s="82" t="s">
@@ -19034,7 +19034,7 @@
         <v>1831</v>
       </c>
       <c r="AN33" s="84" t="s">
-        <v>1949</v>
+        <v>1947</v>
       </c>
       <c r="AO33" s="72"/>
       <c r="AP33" s="82" t="s">
@@ -19044,7 +19044,7 @@
         <v>1831</v>
       </c>
       <c r="AR33" s="84" t="s">
-        <v>1950</v>
+        <v>1948</v>
       </c>
       <c r="AS33" s="72"/>
       <c r="AT33" s="82" t="s">
@@ -19054,7 +19054,7 @@
         <v>1831</v>
       </c>
       <c r="AV33" s="84" t="s">
-        <v>2257</v>
+        <v>2374</v>
       </c>
       <c r="AW33" s="65"/>
     </row>
@@ -19066,7 +19066,7 @@
         <v>1832</v>
       </c>
       <c r="D34" s="84" t="s">
-        <v>1951</v>
+        <v>1949</v>
       </c>
       <c r="E34" s="72"/>
       <c r="F34" s="82" t="s">
@@ -19076,7 +19076,7 @@
         <v>1832</v>
       </c>
       <c r="H34" s="84" t="s">
-        <v>1952</v>
+        <v>1950</v>
       </c>
       <c r="I34" s="72"/>
       <c r="J34" s="82" t="s">
@@ -19086,7 +19086,7 @@
         <v>1832</v>
       </c>
       <c r="L34" s="84" t="s">
-        <v>1953</v>
+        <v>1951</v>
       </c>
       <c r="M34" s="72"/>
       <c r="N34" s="82" t="s">
@@ -19096,7 +19096,7 @@
         <v>1832</v>
       </c>
       <c r="P34" s="84" t="s">
-        <v>2194</v>
+        <v>2186</v>
       </c>
       <c r="Q34" s="72"/>
       <c r="R34" s="82" t="s">
@@ -19106,7 +19106,7 @@
         <v>1832</v>
       </c>
       <c r="T34" s="84" t="s">
-        <v>1954</v>
+        <v>1952</v>
       </c>
       <c r="U34" s="72"/>
       <c r="V34" s="82" t="s">
@@ -19116,7 +19116,7 @@
         <v>1832</v>
       </c>
       <c r="X34" s="84" t="s">
-        <v>2032</v>
+        <v>2028</v>
       </c>
       <c r="Y34" s="72"/>
       <c r="Z34" s="82" t="s">
@@ -19126,7 +19126,7 @@
         <v>1832</v>
       </c>
       <c r="AB34" s="84" t="s">
-        <v>2227</v>
+        <v>2378</v>
       </c>
       <c r="AC34" s="72"/>
       <c r="AD34" s="82" t="s">
@@ -19136,7 +19136,7 @@
         <v>1832</v>
       </c>
       <c r="AF34" s="84" t="s">
-        <v>2012</v>
+        <v>2009</v>
       </c>
       <c r="AG34" s="72"/>
       <c r="AH34" s="82" t="s">
@@ -19146,7 +19146,7 @@
         <v>1832</v>
       </c>
       <c r="AJ34" s="84" t="s">
-        <v>1955</v>
+        <v>1953</v>
       </c>
       <c r="AK34" s="72"/>
       <c r="AL34" s="82" t="s">
@@ -19156,7 +19156,7 @@
         <v>1832</v>
       </c>
       <c r="AN34" s="84" t="s">
-        <v>2294</v>
+        <v>2280</v>
       </c>
       <c r="AO34" s="72"/>
       <c r="AP34" s="82" t="s">
@@ -19166,7 +19166,7 @@
         <v>1832</v>
       </c>
       <c r="AR34" s="84" t="s">
-        <v>1956</v>
+        <v>1954</v>
       </c>
       <c r="AS34" s="72"/>
       <c r="AT34" s="82" t="s">
@@ -19176,7 +19176,7 @@
         <v>1832</v>
       </c>
       <c r="AV34" s="84" t="s">
-        <v>2271</v>
+        <v>2258</v>
       </c>
       <c r="AW34" s="65"/>
     </row>
@@ -19188,7 +19188,7 @@
         <v>1833</v>
       </c>
       <c r="D35" s="84" t="s">
-        <v>1957</v>
+        <v>1955</v>
       </c>
       <c r="E35" s="72"/>
       <c r="F35" s="82" t="s">
@@ -19198,7 +19198,7 @@
         <v>1833</v>
       </c>
       <c r="H35" s="84" t="s">
-        <v>1958</v>
+        <v>1956</v>
       </c>
       <c r="I35" s="72"/>
       <c r="J35" s="82" t="s">
@@ -19208,7 +19208,7 @@
         <v>1833</v>
       </c>
       <c r="L35" s="84" t="s">
-        <v>2243</v>
+        <v>2232</v>
       </c>
       <c r="M35" s="72"/>
       <c r="N35" s="82" t="s">
@@ -19218,7 +19218,7 @@
         <v>1833</v>
       </c>
       <c r="P35" s="84" t="s">
-        <v>2182</v>
+        <v>2175</v>
       </c>
       <c r="Q35" s="72"/>
       <c r="R35" s="82" t="s">
@@ -19228,7 +19228,7 @@
         <v>1833</v>
       </c>
       <c r="T35" s="84" t="s">
-        <v>1885</v>
+        <v>1884</v>
       </c>
       <c r="U35" s="72"/>
       <c r="V35" s="82" t="s">
@@ -19238,7 +19238,7 @@
         <v>1833</v>
       </c>
       <c r="X35" s="84" t="s">
-        <v>1959</v>
+        <v>1957</v>
       </c>
       <c r="Y35" s="72"/>
       <c r="Z35" s="82" t="s">
@@ -19248,7 +19248,7 @@
         <v>1833</v>
       </c>
       <c r="AB35" s="84" t="s">
-        <v>2215</v>
+        <v>2205</v>
       </c>
       <c r="AC35" s="72"/>
       <c r="AD35" s="82" t="s">
@@ -19258,7 +19258,7 @@
         <v>1833</v>
       </c>
       <c r="AF35" s="84" t="s">
-        <v>2378</v>
+        <v>2357</v>
       </c>
       <c r="AG35" s="72"/>
       <c r="AH35" s="82" t="s">
@@ -19268,7 +19268,7 @@
         <v>1833</v>
       </c>
       <c r="AJ35" s="84" t="s">
-        <v>1960</v>
+        <v>1958</v>
       </c>
       <c r="AK35" s="72"/>
       <c r="AL35" s="82" t="s">
@@ -19278,7 +19278,7 @@
         <v>1833</v>
       </c>
       <c r="AN35" s="84" t="s">
-        <v>1961</v>
+        <v>1959</v>
       </c>
       <c r="AO35" s="72"/>
       <c r="AP35" s="82" t="s">
@@ -19288,7 +19288,7 @@
         <v>1833</v>
       </c>
       <c r="AR35" s="84" t="s">
-        <v>2285</v>
+        <v>2238</v>
       </c>
       <c r="AS35" s="72"/>
       <c r="AT35" s="82" t="s">
@@ -19298,7 +19298,7 @@
         <v>1833</v>
       </c>
       <c r="AV35" s="84" t="s">
-        <v>2258</v>
+        <v>2246</v>
       </c>
       <c r="AW35" s="65"/>
     </row>
@@ -19314,7 +19314,7 @@
         <v>1834</v>
       </c>
       <c r="H36" s="84" t="s">
-        <v>1963</v>
+        <v>1961</v>
       </c>
       <c r="I36" s="72"/>
       <c r="J36" s="82" t="s">
@@ -19324,7 +19324,7 @@
         <v>1834</v>
       </c>
       <c r="L36" s="84" t="s">
-        <v>1964</v>
+        <v>1962</v>
       </c>
       <c r="M36" s="72"/>
       <c r="N36" s="82" t="s">
@@ -19334,7 +19334,7 @@
         <v>1834</v>
       </c>
       <c r="P36" s="84" t="s">
-        <v>2314</v>
+        <v>2299</v>
       </c>
       <c r="Q36" s="72"/>
       <c r="R36" s="82" t="s">
@@ -19344,7 +19344,7 @@
         <v>1834</v>
       </c>
       <c r="T36" s="84" t="s">
-        <v>2200</v>
+        <v>2191</v>
       </c>
       <c r="U36" s="72"/>
       <c r="V36" s="82" t="s">
@@ -19354,7 +19354,7 @@
         <v>1834</v>
       </c>
       <c r="X36" s="84" t="s">
-        <v>2205</v>
+        <v>2196</v>
       </c>
       <c r="Y36" s="72"/>
       <c r="Z36" s="82" t="s">
@@ -19364,7 +19364,7 @@
         <v>1834</v>
       </c>
       <c r="AB36" s="84" t="s">
-        <v>2216</v>
+        <v>2206</v>
       </c>
       <c r="AC36" s="72"/>
       <c r="AD36" s="82" t="s">
@@ -19374,7 +19374,7 @@
         <v>1834</v>
       </c>
       <c r="AF36" s="84" t="s">
-        <v>2232</v>
+        <v>2221</v>
       </c>
       <c r="AG36" s="72"/>
       <c r="AH36" s="82" t="s">
@@ -19384,7 +19384,7 @@
         <v>1834</v>
       </c>
       <c r="AJ36" s="84" t="s">
-        <v>2286</v>
+        <v>2272</v>
       </c>
       <c r="AK36" s="72"/>
       <c r="AL36" s="82" t="s">
@@ -19394,7 +19394,7 @@
         <v>1834</v>
       </c>
       <c r="AN36" s="84" t="s">
-        <v>2296</v>
+        <v>2282</v>
       </c>
       <c r="AO36" s="72"/>
       <c r="AP36" s="82" t="s">
@@ -19404,7 +19404,7 @@
         <v>1834</v>
       </c>
       <c r="AR36" s="84" t="s">
-        <v>2287</v>
+        <v>2273</v>
       </c>
       <c r="AS36" s="72"/>
       <c r="AT36" s="82" t="s">
@@ -19414,7 +19414,7 @@
         <v>1834</v>
       </c>
       <c r="AV36" s="84" t="s">
-        <v>2273</v>
+        <v>2260</v>
       </c>
       <c r="AW36" s="65"/>
     </row>
@@ -19426,7 +19426,7 @@
         <v>1835</v>
       </c>
       <c r="D37" s="84" t="s">
-        <v>2228</v>
+        <v>2217</v>
       </c>
       <c r="E37" s="72"/>
       <c r="F37" s="82" t="s">
@@ -19436,7 +19436,7 @@
         <v>1835</v>
       </c>
       <c r="H37" s="84" t="s">
-        <v>2336</v>
+        <v>2319</v>
       </c>
       <c r="I37" s="72"/>
       <c r="J37" s="82" t="s">
@@ -19446,7 +19446,7 @@
         <v>1835</v>
       </c>
       <c r="L37" s="84" t="s">
-        <v>2178</v>
+        <v>2171</v>
       </c>
       <c r="M37" s="72"/>
       <c r="N37" s="95"/>
@@ -19460,7 +19460,7 @@
         <v>1835</v>
       </c>
       <c r="T37" s="84" t="s">
-        <v>1965</v>
+        <v>1963</v>
       </c>
       <c r="U37" s="72"/>
       <c r="V37" s="82" t="s">
@@ -19470,7 +19470,7 @@
         <v>1835</v>
       </c>
       <c r="X37" s="84" t="s">
-        <v>2206</v>
+        <v>2197</v>
       </c>
       <c r="Y37" s="72"/>
       <c r="Z37" s="82" t="s">
@@ -19480,7 +19480,7 @@
         <v>1835</v>
       </c>
       <c r="AB37" s="84" t="s">
-        <v>2217</v>
+        <v>2207</v>
       </c>
       <c r="AC37" s="72"/>
       <c r="AD37" s="82" t="s">
@@ -19490,7 +19490,7 @@
         <v>1835</v>
       </c>
       <c r="AF37" s="84" t="s">
-        <v>2233</v>
+        <v>2222</v>
       </c>
       <c r="AG37" s="72"/>
       <c r="AH37" s="82" t="s">
@@ -19500,7 +19500,7 @@
         <v>1835</v>
       </c>
       <c r="AJ37" s="84" t="s">
-        <v>2315</v>
+        <v>2300</v>
       </c>
       <c r="AK37" s="72"/>
       <c r="AL37" s="82" t="s">
@@ -19510,7 +19510,7 @@
         <v>1835</v>
       </c>
       <c r="AN37" s="84" t="s">
-        <v>2380</v>
+        <v>2359</v>
       </c>
       <c r="AO37" s="72"/>
       <c r="AP37" s="82" t="s">
@@ -19520,7 +19520,7 @@
         <v>1835</v>
       </c>
       <c r="AR37" s="84" t="s">
-        <v>1966</v>
+        <v>2373</v>
       </c>
       <c r="AS37" s="72"/>
       <c r="AT37" s="82" t="s">
@@ -19530,7 +19530,7 @@
         <v>1835</v>
       </c>
       <c r="AV37" s="84" t="s">
-        <v>1967</v>
+        <v>1964</v>
       </c>
       <c r="AW37" s="65"/>
     </row>
@@ -19542,7 +19542,7 @@
         <v>1836</v>
       </c>
       <c r="D38" s="84" t="s">
-        <v>2158</v>
+        <v>2152</v>
       </c>
       <c r="E38" s="72"/>
       <c r="F38" s="82" t="s">
@@ -19552,7 +19552,7 @@
         <v>1836</v>
       </c>
       <c r="H38" s="84" t="s">
-        <v>1939</v>
+        <v>1938</v>
       </c>
       <c r="I38" s="72"/>
       <c r="J38" s="82" t="s">
@@ -19562,7 +19562,7 @@
         <v>1836</v>
       </c>
       <c r="L38" s="84" t="s">
-        <v>1988</v>
+        <v>1985</v>
       </c>
       <c r="M38" s="72"/>
       <c r="N38" s="82" t="s">
@@ -19572,7 +19572,7 @@
         <v>1836</v>
       </c>
       <c r="P38" s="84" t="s">
-        <v>2183</v>
+        <v>2176</v>
       </c>
       <c r="Q38" s="72"/>
       <c r="R38" s="82" t="s">
@@ -19582,7 +19582,7 @@
         <v>1836</v>
       </c>
       <c r="T38" s="84" t="s">
-        <v>2303</v>
+        <v>2289</v>
       </c>
       <c r="U38" s="72"/>
       <c r="V38" s="82" t="s">
@@ -19592,7 +19592,7 @@
         <v>1836</v>
       </c>
       <c r="X38" s="84" t="s">
-        <v>1940</v>
+        <v>1939</v>
       </c>
       <c r="Y38" s="72"/>
       <c r="Z38" s="82" t="s">
@@ -19602,7 +19602,7 @@
         <v>1836</v>
       </c>
       <c r="AB38" s="84" t="s">
-        <v>1968</v>
+        <v>1965</v>
       </c>
       <c r="AC38" s="72"/>
       <c r="AD38" s="82" t="s">
@@ -19612,7 +19612,7 @@
         <v>1836</v>
       </c>
       <c r="AF38" s="84" t="s">
-        <v>2234</v>
+        <v>2223</v>
       </c>
       <c r="AG38" s="72"/>
       <c r="AH38" s="82" t="s">
@@ -19622,7 +19622,7 @@
         <v>1836</v>
       </c>
       <c r="AJ38" s="84" t="s">
-        <v>2309</v>
+        <v>2294</v>
       </c>
       <c r="AK38" s="72"/>
       <c r="AL38" s="82" t="s">
@@ -19632,7 +19632,7 @@
         <v>1836</v>
       </c>
       <c r="AN38" s="84" t="s">
-        <v>2246</v>
+        <v>2235</v>
       </c>
       <c r="AO38" s="72"/>
       <c r="AP38" s="82" t="s">
@@ -19642,7 +19642,7 @@
         <v>1836</v>
       </c>
       <c r="AR38" s="84" t="s">
-        <v>2289</v>
+        <v>2275</v>
       </c>
       <c r="AS38" s="72"/>
       <c r="AT38" s="82" t="s">
@@ -19652,7 +19652,7 @@
         <v>1836</v>
       </c>
       <c r="AV38" s="84" t="s">
-        <v>2259</v>
+        <v>2247</v>
       </c>
       <c r="AW38" s="65"/>
     </row>
@@ -19664,7 +19664,7 @@
         <v>1837</v>
       </c>
       <c r="D39" s="84" t="s">
-        <v>2161</v>
+        <v>2367</v>
       </c>
       <c r="E39" s="72"/>
       <c r="F39" s="82" t="s">
@@ -19674,7 +19674,7 @@
         <v>1837</v>
       </c>
       <c r="H39" s="84" t="s">
-        <v>2164</v>
+        <v>2157</v>
       </c>
       <c r="I39" s="72"/>
       <c r="J39" s="82" t="s">
@@ -19684,7 +19684,7 @@
         <v>1837</v>
       </c>
       <c r="L39" s="84" t="s">
-        <v>1970</v>
+        <v>1967</v>
       </c>
       <c r="M39" s="72"/>
       <c r="N39" s="82" t="s">
@@ -19694,7 +19694,7 @@
         <v>1837</v>
       </c>
       <c r="P39" s="84" t="s">
-        <v>2184</v>
+        <v>2177</v>
       </c>
       <c r="Q39" s="72"/>
       <c r="R39" s="82" t="s">
@@ -19704,7 +19704,7 @@
         <v>1837</v>
       </c>
       <c r="T39" s="84" t="s">
-        <v>1971</v>
+        <v>1968</v>
       </c>
       <c r="U39" s="72"/>
       <c r="V39" s="82" t="s">
@@ -19714,7 +19714,7 @@
         <v>1837</v>
       </c>
       <c r="X39" s="84" t="s">
-        <v>2319</v>
+        <v>2304</v>
       </c>
       <c r="Y39" s="72"/>
       <c r="Z39" s="82" t="s">
@@ -19724,7 +19724,7 @@
         <v>1837</v>
       </c>
       <c r="AB39" s="84" t="s">
-        <v>2348</v>
+        <v>2379</v>
       </c>
       <c r="AC39" s="72"/>
       <c r="AD39" s="82" t="s">
@@ -19734,7 +19734,7 @@
         <v>1837</v>
       </c>
       <c r="AF39" s="84" t="s">
-        <v>2343</v>
+        <v>2326</v>
       </c>
       <c r="AG39" s="72"/>
       <c r="AH39" s="82" t="s">
@@ -19744,7 +19744,7 @@
         <v>1837</v>
       </c>
       <c r="AJ39" s="84" t="s">
-        <v>1972</v>
+        <v>1969</v>
       </c>
       <c r="AK39" s="72"/>
       <c r="AL39" s="82" t="s">
@@ -19754,7 +19754,7 @@
         <v>1837</v>
       </c>
       <c r="AN39" s="84" t="s">
-        <v>1973</v>
+        <v>1970</v>
       </c>
       <c r="AO39" s="72"/>
       <c r="AP39" s="82" t="s">
@@ -19764,7 +19764,7 @@
         <v>1837</v>
       </c>
       <c r="AR39" s="84" t="s">
-        <v>2055</v>
+        <v>2051</v>
       </c>
       <c r="AS39" s="72"/>
       <c r="AT39" s="82" t="s">
@@ -19774,7 +19774,7 @@
         <v>1837</v>
       </c>
       <c r="AV39" s="84" t="s">
-        <v>2383</v>
+        <v>2362</v>
       </c>
       <c r="AW39" s="65"/>
     </row>
@@ -19790,7 +19790,7 @@
         <v>1838</v>
       </c>
       <c r="H40" s="81" t="s">
-        <v>2165</v>
+        <v>2158</v>
       </c>
       <c r="I40" s="72"/>
       <c r="J40" s="82" t="s">
@@ -19800,7 +19800,7 @@
         <v>1838</v>
       </c>
       <c r="L40" s="84" t="s">
-        <v>2385</v>
+        <v>2364</v>
       </c>
       <c r="M40" s="72"/>
       <c r="N40" s="82" t="s">
@@ -19810,7 +19810,7 @@
         <v>1838</v>
       </c>
       <c r="P40" s="84" t="s">
-        <v>2185</v>
+        <v>2178</v>
       </c>
       <c r="Q40" s="72"/>
       <c r="R40" s="82" t="s">
@@ -19820,7 +19820,7 @@
         <v>1838</v>
       </c>
       <c r="T40" s="84" t="s">
-        <v>2025</v>
+        <v>2021</v>
       </c>
       <c r="U40" s="72"/>
       <c r="V40" s="82" t="s">
@@ -19830,7 +19830,7 @@
         <v>1838</v>
       </c>
       <c r="X40" s="84" t="s">
-        <v>2213</v>
+        <v>2203</v>
       </c>
       <c r="Y40" s="72"/>
       <c r="Z40" s="82" t="s">
@@ -19840,7 +19840,7 @@
         <v>1838</v>
       </c>
       <c r="AB40" s="84" t="s">
-        <v>1974</v>
+        <v>1971</v>
       </c>
       <c r="AC40" s="72"/>
       <c r="AD40" s="82" t="s">
@@ -19850,7 +19850,7 @@
         <v>1838</v>
       </c>
       <c r="AF40" s="84" t="s">
-        <v>1975</v>
+        <v>1972</v>
       </c>
       <c r="AG40" s="72"/>
       <c r="AH40" s="82" t="s">
@@ -19860,7 +19860,7 @@
         <v>1838</v>
       </c>
       <c r="AJ40" s="84" t="s">
-        <v>1976</v>
+        <v>1973</v>
       </c>
       <c r="AK40" s="72"/>
       <c r="AL40" s="82" t="s">
@@ -19870,7 +19870,7 @@
         <v>1838</v>
       </c>
       <c r="AN40" s="84" t="s">
-        <v>2297</v>
+        <v>2283</v>
       </c>
       <c r="AO40" s="72"/>
       <c r="AP40" s="82" t="s">
@@ -19880,7 +19880,7 @@
         <v>1838</v>
       </c>
       <c r="AR40" s="84" t="s">
-        <v>2290</v>
+        <v>2276</v>
       </c>
       <c r="AS40" s="72"/>
       <c r="AT40" s="82" t="s">
@@ -19890,7 +19890,7 @@
         <v>1838</v>
       </c>
       <c r="AV40" s="84" t="s">
-        <v>2260</v>
+        <v>2248</v>
       </c>
       <c r="AW40" s="65"/>
     </row>
@@ -19902,7 +19902,7 @@
         <v>1839</v>
       </c>
       <c r="D41" s="81" t="s">
-        <v>1977</v>
+        <v>1974</v>
       </c>
       <c r="E41" s="72"/>
       <c r="F41" s="82"/>
@@ -19916,7 +19916,7 @@
         <v>1839</v>
       </c>
       <c r="L41" s="84" t="s">
-        <v>2334</v>
+        <v>2318</v>
       </c>
       <c r="M41" s="72"/>
       <c r="N41" s="82" t="s">
@@ -19926,7 +19926,7 @@
         <v>1839</v>
       </c>
       <c r="P41" s="84" t="s">
-        <v>2186</v>
+        <v>2179</v>
       </c>
       <c r="Q41" s="72"/>
       <c r="R41" s="82" t="s">
@@ -19936,7 +19936,7 @@
         <v>1839</v>
       </c>
       <c r="T41" s="84" t="s">
-        <v>1991</v>
+        <v>1988</v>
       </c>
       <c r="U41" s="72"/>
       <c r="V41" s="82" t="s">
@@ -19946,7 +19946,7 @@
         <v>1839</v>
       </c>
       <c r="X41" s="84" t="s">
-        <v>2318</v>
+        <v>2303</v>
       </c>
       <c r="Y41" s="72"/>
       <c r="Z41" s="82" t="s">
@@ -19956,7 +19956,7 @@
         <v>1839</v>
       </c>
       <c r="AB41" s="84" t="s">
-        <v>2317</v>
+        <v>2302</v>
       </c>
       <c r="AC41" s="72"/>
       <c r="AD41" s="82" t="s">
@@ -19966,7 +19966,7 @@
         <v>1839</v>
       </c>
       <c r="AF41" s="84" t="s">
-        <v>2235</v>
+        <v>2224</v>
       </c>
       <c r="AG41" s="72"/>
       <c r="AH41" s="82" t="s">
@@ -19976,7 +19976,7 @@
         <v>1839</v>
       </c>
       <c r="AJ41" s="84" t="s">
-        <v>2244</v>
+        <v>2233</v>
       </c>
       <c r="AK41" s="72"/>
       <c r="AL41" s="82" t="s">
@@ -19986,7 +19986,7 @@
         <v>1839</v>
       </c>
       <c r="AN41" s="84" t="s">
-        <v>1979</v>
+        <v>1976</v>
       </c>
       <c r="AO41" s="72"/>
       <c r="AP41" s="82" t="s">
@@ -19996,7 +19996,7 @@
         <v>1839</v>
       </c>
       <c r="AR41" s="84" t="s">
-        <v>1980</v>
+        <v>1977</v>
       </c>
       <c r="AS41" s="72"/>
       <c r="AT41" s="82" t="s">
@@ -20006,7 +20006,7 @@
         <v>1839</v>
       </c>
       <c r="AV41" s="84" t="s">
-        <v>2261</v>
+        <v>2249</v>
       </c>
       <c r="AW41" s="65"/>
     </row>
@@ -20018,7 +20018,7 @@
         <v>1840</v>
       </c>
       <c r="D42" s="84" t="s">
-        <v>2369</v>
+        <v>2349</v>
       </c>
       <c r="E42" s="72"/>
       <c r="F42" s="82" t="s">
@@ -20028,7 +20028,7 @@
         <v>1840</v>
       </c>
       <c r="H42" s="84" t="s">
-        <v>2281</v>
+        <v>2268</v>
       </c>
       <c r="I42" s="72"/>
       <c r="J42" s="82"/>
@@ -20042,7 +20042,7 @@
         <v>1840</v>
       </c>
       <c r="P42" s="81" t="s">
-        <v>2187</v>
+        <v>2180</v>
       </c>
       <c r="Q42" s="72"/>
       <c r="R42" s="82" t="s">
@@ -20052,7 +20052,7 @@
         <v>1840</v>
       </c>
       <c r="T42" s="84" t="s">
-        <v>2375</v>
+        <v>2355</v>
       </c>
       <c r="U42" s="72"/>
       <c r="V42" s="82" t="s">
@@ -20062,7 +20062,7 @@
         <v>1840</v>
       </c>
       <c r="X42" s="84" t="s">
-        <v>1978</v>
+        <v>1975</v>
       </c>
       <c r="Y42" s="72"/>
       <c r="Z42" s="82" t="s">
@@ -20072,7 +20072,7 @@
         <v>1840</v>
       </c>
       <c r="AB42" s="84" t="s">
-        <v>2218</v>
+        <v>2208</v>
       </c>
       <c r="AC42" s="72"/>
       <c r="AD42" s="82" t="s">
@@ -20082,7 +20082,7 @@
         <v>1840</v>
       </c>
       <c r="AF42" s="84" t="s">
-        <v>1982</v>
+        <v>1979</v>
       </c>
       <c r="AG42" s="72"/>
       <c r="AH42" s="82" t="s">
@@ -20092,7 +20092,7 @@
         <v>1840</v>
       </c>
       <c r="AJ42" s="84" t="s">
-        <v>2313</v>
+        <v>2298</v>
       </c>
       <c r="AK42" s="72"/>
       <c r="AL42" s="82" t="s">
@@ -20102,7 +20102,7 @@
         <v>1840</v>
       </c>
       <c r="AN42" s="84" t="s">
-        <v>1983</v>
+        <v>1980</v>
       </c>
       <c r="AO42" s="72"/>
       <c r="AP42" s="82" t="s">
@@ -20112,7 +20112,7 @@
         <v>1840</v>
       </c>
       <c r="AR42" s="84" t="s">
-        <v>2251</v>
+        <v>2240</v>
       </c>
       <c r="AS42" s="72"/>
       <c r="AT42" s="82" t="s">
@@ -20122,7 +20122,7 @@
         <v>1840</v>
       </c>
       <c r="AV42" s="84" t="s">
-        <v>2262</v>
+        <v>2250</v>
       </c>
     </row>
     <row r="43" spans="2:49">
@@ -20133,7 +20133,7 @@
         <v>1841</v>
       </c>
       <c r="D43" s="84" t="s">
-        <v>2370</v>
+        <v>2350</v>
       </c>
       <c r="E43" s="72"/>
       <c r="F43" s="82" t="s">
@@ -20143,7 +20143,7 @@
         <v>1841</v>
       </c>
       <c r="H43" s="84" t="s">
-        <v>2166</v>
+        <v>2159</v>
       </c>
       <c r="I43" s="72"/>
       <c r="J43" s="79" t="s">
@@ -20153,7 +20153,7 @@
         <v>1841</v>
       </c>
       <c r="L43" s="81" t="s">
-        <v>2335</v>
+        <v>2370</v>
       </c>
       <c r="M43" s="72"/>
       <c r="N43" s="82"/>
@@ -20167,7 +20167,7 @@
         <v>1841</v>
       </c>
       <c r="T43" s="81" t="s">
-        <v>2201</v>
+        <v>2192</v>
       </c>
       <c r="U43" s="72"/>
       <c r="V43" s="79" t="s">
@@ -20177,7 +20177,7 @@
         <v>1841</v>
       </c>
       <c r="X43" s="81" t="s">
-        <v>1984</v>
+        <v>1981</v>
       </c>
       <c r="Y43" s="72"/>
       <c r="Z43" s="82" t="s">
@@ -20187,7 +20187,7 @@
         <v>1841</v>
       </c>
       <c r="AB43" s="84" t="s">
-        <v>2219</v>
+        <v>2209</v>
       </c>
       <c r="AC43" s="72"/>
       <c r="AD43" s="82" t="s">
@@ -20197,7 +20197,7 @@
         <v>1841</v>
       </c>
       <c r="AF43" s="84" t="s">
-        <v>2236</v>
+        <v>2225</v>
       </c>
       <c r="AG43" s="72"/>
       <c r="AH43" s="82" t="s">
@@ -20207,7 +20207,7 @@
         <v>1841</v>
       </c>
       <c r="AJ43" s="84" t="s">
-        <v>2316</v>
+        <v>2301</v>
       </c>
       <c r="AK43" s="72"/>
       <c r="AL43" s="82" t="s">
@@ -20217,7 +20217,7 @@
         <v>1841</v>
       </c>
       <c r="AN43" s="84" t="s">
-        <v>2298</v>
+        <v>2284</v>
       </c>
       <c r="AO43" s="72"/>
       <c r="AP43" s="82" t="s">
@@ -20227,7 +20227,7 @@
         <v>1841</v>
       </c>
       <c r="AR43" s="84" t="s">
-        <v>1985</v>
+        <v>1982</v>
       </c>
       <c r="AS43" s="72"/>
       <c r="AT43" s="82" t="s">
@@ -20237,7 +20237,7 @@
         <v>1841</v>
       </c>
       <c r="AV43" s="84" t="s">
-        <v>2275</v>
+        <v>2262</v>
       </c>
       <c r="AW43" s="65"/>
     </row>
@@ -20249,7 +20249,7 @@
         <v>1842</v>
       </c>
       <c r="D44" s="84" t="s">
-        <v>1986</v>
+        <v>1983</v>
       </c>
       <c r="E44" s="72"/>
       <c r="F44" s="82" t="s">
@@ -20259,7 +20259,7 @@
         <v>1842</v>
       </c>
       <c r="H44" s="84" t="s">
-        <v>1987</v>
+        <v>1984</v>
       </c>
       <c r="I44" s="72"/>
       <c r="J44" s="82" t="s">
@@ -20269,7 +20269,7 @@
         <v>1842</v>
       </c>
       <c r="L44" s="84" t="s">
-        <v>2323</v>
+        <v>2308</v>
       </c>
       <c r="M44" s="72"/>
       <c r="N44" s="82" t="s">
@@ -20279,7 +20279,7 @@
         <v>1842</v>
       </c>
       <c r="P44" s="84" t="s">
-        <v>2188</v>
+        <v>2181</v>
       </c>
       <c r="Q44" s="72"/>
       <c r="R44" s="82"/>
@@ -20293,7 +20293,7 @@
         <v>1842</v>
       </c>
       <c r="X44" s="81" t="s">
-        <v>2377</v>
+        <v>2383</v>
       </c>
       <c r="Y44" s="72"/>
       <c r="Z44" s="82" t="s">
@@ -20303,7 +20303,7 @@
         <v>1842</v>
       </c>
       <c r="AB44" s="84" t="s">
-        <v>1989</v>
+        <v>1986</v>
       </c>
       <c r="AC44" s="72"/>
       <c r="AD44" s="82" t="s">
@@ -20313,7 +20313,7 @@
         <v>1842</v>
       </c>
       <c r="AF44" s="84" t="s">
-        <v>2237</v>
+        <v>2226</v>
       </c>
       <c r="AG44" s="72"/>
       <c r="AH44" s="82" t="s">
@@ -20323,7 +20323,7 @@
         <v>1842</v>
       </c>
       <c r="AJ44" s="84" t="s">
-        <v>1990</v>
+        <v>1987</v>
       </c>
       <c r="AK44" s="72"/>
       <c r="AL44" s="82" t="s">
@@ -20333,7 +20333,7 @@
         <v>1842</v>
       </c>
       <c r="AN44" s="84" t="s">
-        <v>2247</v>
+        <v>2236</v>
       </c>
       <c r="AO44" s="72"/>
       <c r="AP44" s="82" t="s">
@@ -20343,7 +20343,7 @@
         <v>1842</v>
       </c>
       <c r="AR44" s="84" t="s">
-        <v>2381</v>
+        <v>2360</v>
       </c>
       <c r="AS44" s="72"/>
       <c r="AT44" s="82" t="s">
@@ -20353,7 +20353,7 @@
         <v>1842</v>
       </c>
       <c r="AV44" s="84" t="s">
-        <v>2263</v>
+        <v>2251</v>
       </c>
       <c r="AW44" s="65"/>
     </row>
@@ -20365,7 +20365,7 @@
         <v>1843</v>
       </c>
       <c r="D45" s="84" t="s">
-        <v>2159</v>
+        <v>2153</v>
       </c>
       <c r="E45" s="72"/>
       <c r="F45" s="82" t="s">
@@ -20375,7 +20375,7 @@
         <v>1843</v>
       </c>
       <c r="H45" s="84" t="s">
-        <v>2167</v>
+        <v>2160</v>
       </c>
       <c r="I45" s="72"/>
       <c r="J45" s="82" t="s">
@@ -20385,7 +20385,7 @@
         <v>1843</v>
       </c>
       <c r="L45" s="84" t="s">
-        <v>1992</v>
+        <v>1989</v>
       </c>
       <c r="M45" s="72"/>
       <c r="N45" s="82" t="s">
@@ -20395,7 +20395,7 @@
         <v>1843</v>
       </c>
       <c r="P45" s="84" t="s">
-        <v>2189</v>
+        <v>2182</v>
       </c>
       <c r="Q45" s="72"/>
       <c r="R45" s="79" t="s">
@@ -20405,7 +20405,7 @@
         <v>1843</v>
       </c>
       <c r="T45" s="81" t="s">
-        <v>1993</v>
+        <v>1990</v>
       </c>
       <c r="U45" s="72"/>
       <c r="V45" s="82"/>
@@ -20419,7 +20419,7 @@
         <v>1843</v>
       </c>
       <c r="AB45" s="84" t="s">
-        <v>2220</v>
+        <v>2210</v>
       </c>
       <c r="AC45" s="72"/>
       <c r="AD45" s="82" t="s">
@@ -20429,7 +20429,7 @@
         <v>1843</v>
       </c>
       <c r="AF45" s="84" t="s">
-        <v>2238</v>
+        <v>2227</v>
       </c>
       <c r="AG45" s="72"/>
       <c r="AH45" s="82" t="s">
@@ -20439,7 +20439,7 @@
         <v>1843</v>
       </c>
       <c r="AJ45" s="84" t="s">
-        <v>1994</v>
+        <v>1991</v>
       </c>
       <c r="AK45" s="72"/>
       <c r="AL45" s="82" t="s">
@@ -20449,7 +20449,7 @@
         <v>1843</v>
       </c>
       <c r="AN45" s="84" t="s">
-        <v>2116</v>
+        <v>2110</v>
       </c>
       <c r="AO45" s="72"/>
       <c r="AP45" s="82" t="s">
@@ -20459,7 +20459,7 @@
         <v>1843</v>
       </c>
       <c r="AR45" s="84" t="s">
-        <v>1995</v>
+        <v>1992</v>
       </c>
       <c r="AS45" s="72"/>
       <c r="AT45" s="82" t="s">
@@ -20469,7 +20469,7 @@
         <v>1843</v>
       </c>
       <c r="AV45" s="84" t="s">
-        <v>2265</v>
+        <v>2375</v>
       </c>
       <c r="AW45" s="65"/>
     </row>
@@ -20481,7 +20481,7 @@
         <v>1844</v>
       </c>
       <c r="D46" s="84" t="s">
-        <v>2371</v>
+        <v>2351</v>
       </c>
       <c r="E46" s="72"/>
       <c r="F46" s="82" t="s">
@@ -20491,7 +20491,7 @@
         <v>1844</v>
       </c>
       <c r="H46" s="84" t="s">
-        <v>2337</v>
+        <v>2320</v>
       </c>
       <c r="I46" s="72"/>
       <c r="J46" s="82" t="s">
@@ -20501,7 +20501,7 @@
         <v>1844</v>
       </c>
       <c r="L46" s="84" t="s">
-        <v>1996</v>
+        <v>1993</v>
       </c>
       <c r="M46" s="72"/>
       <c r="N46" s="82" t="s">
@@ -20511,7 +20511,7 @@
         <v>1844</v>
       </c>
       <c r="P46" s="84" t="s">
-        <v>2190</v>
+        <v>2183</v>
       </c>
       <c r="Q46" s="72"/>
       <c r="R46" s="82" t="s">
@@ -20521,7 +20521,7 @@
         <v>1844</v>
       </c>
       <c r="T46" s="84" t="s">
-        <v>1997</v>
+        <v>1994</v>
       </c>
       <c r="U46" s="72"/>
       <c r="V46" s="82" t="s">
@@ -20531,7 +20531,7 @@
         <v>1844</v>
       </c>
       <c r="X46" s="84" t="s">
-        <v>2207</v>
+        <v>2198</v>
       </c>
       <c r="Y46" s="72"/>
       <c r="Z46" s="82"/>
@@ -20545,7 +20545,7 @@
         <v>1844</v>
       </c>
       <c r="AF46" s="81" t="s">
-        <v>1998</v>
+        <v>1995</v>
       </c>
       <c r="AG46" s="72"/>
       <c r="AH46" s="82" t="s">
@@ -20555,7 +20555,7 @@
         <v>1844</v>
       </c>
       <c r="AJ46" s="84" t="s">
-        <v>2208</v>
+        <v>2199</v>
       </c>
       <c r="AK46" s="72"/>
       <c r="AL46" s="82" t="s">
@@ -20565,7 +20565,7 @@
         <v>1844</v>
       </c>
       <c r="AN46" s="84" t="s">
-        <v>1999</v>
+        <v>1996</v>
       </c>
       <c r="AO46" s="72"/>
       <c r="AP46" s="82" t="s">
@@ -20575,7 +20575,7 @@
         <v>1844</v>
       </c>
       <c r="AR46" s="84" t="s">
-        <v>2291</v>
+        <v>2277</v>
       </c>
       <c r="AS46" s="72"/>
       <c r="AT46" s="82" t="s">
@@ -20585,7 +20585,7 @@
         <v>1844</v>
       </c>
       <c r="AV46" s="84" t="s">
-        <v>2264</v>
+        <v>2252</v>
       </c>
       <c r="AW46" s="65"/>
     </row>
@@ -20597,7 +20597,7 @@
         <v>1845</v>
       </c>
       <c r="D47" s="84" t="s">
-        <v>2160</v>
+        <v>2154</v>
       </c>
       <c r="E47" s="72"/>
       <c r="F47" s="82" t="s">
@@ -20607,7 +20607,7 @@
         <v>1845</v>
       </c>
       <c r="H47" s="84" t="s">
-        <v>2332</v>
+        <v>2385</v>
       </c>
       <c r="I47" s="72"/>
       <c r="J47" s="82" t="s">
@@ -20617,7 +20617,7 @@
         <v>1845</v>
       </c>
       <c r="L47" s="84" t="s">
-        <v>2179</v>
+        <v>2172</v>
       </c>
       <c r="M47" s="72"/>
       <c r="N47" s="82" t="s">
@@ -20627,7 +20627,7 @@
         <v>1845</v>
       </c>
       <c r="P47" s="84" t="s">
-        <v>2191</v>
+        <v>2184</v>
       </c>
       <c r="Q47" s="72"/>
       <c r="R47" s="82" t="s">
@@ -20637,7 +20637,7 @@
         <v>1845</v>
       </c>
       <c r="T47" s="84" t="s">
-        <v>2330</v>
+        <v>2315</v>
       </c>
       <c r="U47" s="72"/>
       <c r="V47" s="82" t="s">
@@ -20647,7 +20647,7 @@
         <v>1845</v>
       </c>
       <c r="X47" s="84" t="s">
-        <v>2209</v>
+        <v>2200</v>
       </c>
       <c r="Y47" s="72"/>
       <c r="Z47" s="79" t="s">
@@ -20657,7 +20657,7 @@
         <v>1845</v>
       </c>
       <c r="AB47" s="81" t="s">
-        <v>2221</v>
+        <v>2211</v>
       </c>
       <c r="AC47" s="72"/>
       <c r="AD47" s="82"/>
@@ -20671,7 +20671,7 @@
         <v>1845</v>
       </c>
       <c r="AJ47" s="84" t="s">
-        <v>2312</v>
+        <v>2297</v>
       </c>
       <c r="AK47" s="72"/>
       <c r="AL47" s="82" t="s">
@@ -20681,7 +20681,7 @@
         <v>1845</v>
       </c>
       <c r="AN47" s="84" t="s">
-        <v>2248</v>
+        <v>2237</v>
       </c>
       <c r="AO47" s="72"/>
       <c r="AP47" s="82" t="s">
@@ -20691,7 +20691,7 @@
         <v>1845</v>
       </c>
       <c r="AR47" s="84" t="s">
-        <v>2000</v>
+        <v>1997</v>
       </c>
       <c r="AS47" s="72"/>
       <c r="AT47" s="82" t="s">
@@ -20701,7 +20701,7 @@
         <v>1845</v>
       </c>
       <c r="AV47" s="84" t="s">
-        <v>2266</v>
+        <v>2253</v>
       </c>
       <c r="AW47" s="65"/>
     </row>
@@ -20713,7 +20713,7 @@
         <v>1846</v>
       </c>
       <c r="D48" s="84" t="s">
-        <v>2169</v>
+        <v>2162</v>
       </c>
       <c r="E48" s="72"/>
       <c r="F48" s="82" t="s">
@@ -20723,7 +20723,7 @@
         <v>1846</v>
       </c>
       <c r="H48" s="84" t="s">
-        <v>2338</v>
+        <v>2321</v>
       </c>
       <c r="I48" s="72"/>
       <c r="J48" s="82" t="s">
@@ -20733,7 +20733,7 @@
         <v>1846</v>
       </c>
       <c r="L48" s="84" t="s">
-        <v>2180</v>
+        <v>2173</v>
       </c>
       <c r="M48" s="72"/>
       <c r="N48" s="82" t="s">
@@ -20743,7 +20743,7 @@
         <v>1846</v>
       </c>
       <c r="P48" s="84" t="s">
-        <v>2342</v>
+        <v>2325</v>
       </c>
       <c r="Q48" s="72"/>
       <c r="R48" s="82" t="s">
@@ -20753,7 +20753,7 @@
         <v>1846</v>
       </c>
       <c r="T48" s="84" t="s">
-        <v>2376</v>
+        <v>2356</v>
       </c>
       <c r="U48" s="72"/>
       <c r="V48" s="82" t="s">
@@ -20763,7 +20763,7 @@
         <v>1846</v>
       </c>
       <c r="X48" s="84" t="s">
-        <v>2210</v>
+        <v>2201</v>
       </c>
       <c r="Y48" s="72"/>
       <c r="Z48" s="82" t="s">
@@ -20773,7 +20773,7 @@
         <v>1846</v>
       </c>
       <c r="AB48" s="84" t="s">
-        <v>2022</v>
+        <v>2018</v>
       </c>
       <c r="AC48" s="72"/>
       <c r="AD48" s="82" t="s">
@@ -20783,7 +20783,7 @@
         <v>1846</v>
       </c>
       <c r="AF48" s="84" t="s">
-        <v>2344</v>
+        <v>2327</v>
       </c>
       <c r="AG48" s="72"/>
       <c r="AH48" s="82"/>
@@ -20797,7 +20797,7 @@
         <v>1846</v>
       </c>
       <c r="AN48" s="84" t="s">
-        <v>2299</v>
+        <v>2285</v>
       </c>
       <c r="AO48" s="72"/>
       <c r="AP48" s="82" t="s">
@@ -20807,7 +20807,7 @@
         <v>1846</v>
       </c>
       <c r="AR48" s="84" t="s">
-        <v>2382</v>
+        <v>2361</v>
       </c>
       <c r="AS48" s="72"/>
       <c r="AT48" s="82" t="s">
@@ -20817,7 +20817,7 @@
         <v>1846</v>
       </c>
       <c r="AV48" s="84" t="s">
-        <v>2267</v>
+        <v>2254</v>
       </c>
       <c r="AW48" s="65"/>
     </row>
@@ -20829,7 +20829,7 @@
         <v>1847</v>
       </c>
       <c r="D49" s="84" t="s">
-        <v>2372</v>
+        <v>2352</v>
       </c>
       <c r="E49" s="72"/>
       <c r="F49" s="82" t="s">
@@ -20839,7 +20839,7 @@
         <v>1847</v>
       </c>
       <c r="H49" s="84" t="s">
-        <v>2339</v>
+        <v>2322</v>
       </c>
       <c r="I49" s="72"/>
       <c r="J49" s="82" t="s">
@@ -20849,7 +20849,7 @@
         <v>1847</v>
       </c>
       <c r="L49" s="84" t="s">
-        <v>2154</v>
+        <v>2148</v>
       </c>
       <c r="M49" s="72"/>
       <c r="N49" s="82" t="s">
@@ -20859,7 +20859,7 @@
         <v>1847</v>
       </c>
       <c r="P49" s="84" t="s">
-        <v>2224</v>
+        <v>2214</v>
       </c>
       <c r="Q49" s="72"/>
       <c r="R49" s="82" t="s">
@@ -20869,7 +20869,7 @@
         <v>1847</v>
       </c>
       <c r="T49" s="84" t="s">
-        <v>2002</v>
+        <v>1999</v>
       </c>
       <c r="U49" s="72"/>
       <c r="V49" s="82" t="s">
@@ -20879,7 +20879,7 @@
         <v>1847</v>
       </c>
       <c r="X49" s="84" t="s">
-        <v>2003</v>
+        <v>2000</v>
       </c>
       <c r="Y49" s="72"/>
       <c r="Z49" s="82" t="s">
@@ -20889,7 +20889,7 @@
         <v>1847</v>
       </c>
       <c r="AB49" s="84" t="s">
-        <v>2222</v>
+        <v>2212</v>
       </c>
       <c r="AC49" s="72"/>
       <c r="AD49" s="82" t="s">
@@ -20899,7 +20899,7 @@
         <v>1847</v>
       </c>
       <c r="AF49" s="84" t="s">
-        <v>2345</v>
+        <v>2328</v>
       </c>
       <c r="AG49" s="72"/>
       <c r="AH49" s="82" t="s">
@@ -20909,7 +20909,7 @@
         <v>1847</v>
       </c>
       <c r="AJ49" s="84" t="s">
-        <v>2001</v>
+        <v>1998</v>
       </c>
       <c r="AK49" s="72"/>
       <c r="AL49" s="82"/>
@@ -20923,7 +20923,7 @@
         <v>1847</v>
       </c>
       <c r="AR49" s="84" t="s">
-        <v>2004</v>
+        <v>2001</v>
       </c>
       <c r="AS49" s="72"/>
       <c r="AT49" s="82" t="s">
@@ -20933,7 +20933,7 @@
         <v>1847</v>
       </c>
       <c r="AV49" s="84" t="s">
-        <v>2015</v>
+        <v>2012</v>
       </c>
     </row>
     <row r="50" spans="2:49">
@@ -20944,7 +20944,7 @@
         <v>1848</v>
       </c>
       <c r="D50" s="84" t="s">
-        <v>2005</v>
+        <v>2002</v>
       </c>
       <c r="E50" s="72"/>
       <c r="F50" s="82" t="s">
@@ -20954,7 +20954,7 @@
         <v>1848</v>
       </c>
       <c r="H50" s="84" t="s">
-        <v>2340</v>
+        <v>2323</v>
       </c>
       <c r="I50" s="72"/>
       <c r="J50" s="82" t="s">
@@ -20964,7 +20964,7 @@
         <v>1848</v>
       </c>
       <c r="L50" s="84" t="s">
-        <v>2006</v>
+        <v>2003</v>
       </c>
       <c r="M50" s="72"/>
       <c r="N50" s="82" t="s">
@@ -20974,7 +20974,7 @@
         <v>1848</v>
       </c>
       <c r="P50" s="84" t="s">
-        <v>2192</v>
+        <v>2384</v>
       </c>
       <c r="Q50" s="72"/>
       <c r="R50" s="82" t="s">
@@ -20984,7 +20984,7 @@
         <v>1848</v>
       </c>
       <c r="T50" s="84" t="s">
-        <v>2379</v>
+        <v>2358</v>
       </c>
       <c r="U50" s="72"/>
       <c r="V50" s="82" t="s">
@@ -20994,7 +20994,7 @@
         <v>1848</v>
       </c>
       <c r="X50" s="84" t="s">
-        <v>2007</v>
+        <v>2004</v>
       </c>
       <c r="Y50" s="72"/>
       <c r="Z50" s="82" t="s">
@@ -21004,7 +21004,7 @@
         <v>1848</v>
       </c>
       <c r="AB50" s="84" t="s">
-        <v>2223</v>
+        <v>2213</v>
       </c>
       <c r="AC50" s="72"/>
       <c r="AD50" s="82" t="s">
@@ -21014,7 +21014,7 @@
         <v>1848</v>
       </c>
       <c r="AF50" s="84" t="s">
-        <v>2346</v>
+        <v>2329</v>
       </c>
       <c r="AG50" s="72"/>
       <c r="AH50" s="82" t="s">
@@ -21024,7 +21024,7 @@
         <v>1848</v>
       </c>
       <c r="AJ50" s="84" t="s">
-        <v>2008</v>
+        <v>2005</v>
       </c>
       <c r="AK50" s="72"/>
       <c r="AL50" s="82" t="s">
@@ -21034,7 +21034,7 @@
         <v>1848</v>
       </c>
       <c r="AN50" s="84" t="s">
-        <v>2300</v>
+        <v>2286</v>
       </c>
       <c r="AO50" s="72"/>
       <c r="AP50" s="82"/>
@@ -21048,7 +21048,7 @@
         <v>1848</v>
       </c>
       <c r="AV50" s="81" t="s">
-        <v>2268</v>
+        <v>2255</v>
       </c>
       <c r="AW50" s="65"/>
     </row>
@@ -21060,7 +21060,7 @@
         <v>1849</v>
       </c>
       <c r="D51" s="91" t="s">
-        <v>2115</v>
+        <v>2109</v>
       </c>
       <c r="E51" s="72"/>
       <c r="F51" s="89" t="s">
@@ -21070,7 +21070,7 @@
         <v>1849</v>
       </c>
       <c r="H51" s="91" t="s">
-        <v>2301</v>
+        <v>2287</v>
       </c>
       <c r="I51" s="72"/>
       <c r="J51" s="89" t="s">
@@ -21080,7 +21080,7 @@
         <v>1849</v>
       </c>
       <c r="L51" s="91" t="s">
-        <v>2009</v>
+        <v>2006</v>
       </c>
       <c r="M51" s="72"/>
       <c r="N51" s="89" t="s">
@@ -21090,7 +21090,7 @@
         <v>1849</v>
       </c>
       <c r="P51" s="91" t="s">
-        <v>2193</v>
+        <v>2185</v>
       </c>
       <c r="Q51" s="72"/>
       <c r="R51" s="89" t="s">
@@ -21100,7 +21100,7 @@
         <v>1849</v>
       </c>
       <c r="T51" s="91" t="s">
-        <v>2202</v>
+        <v>2193</v>
       </c>
       <c r="U51" s="72"/>
       <c r="V51" s="89" t="s">
@@ -21110,7 +21110,7 @@
         <v>1849</v>
       </c>
       <c r="X51" s="91" t="s">
-        <v>2211</v>
+        <v>2372</v>
       </c>
       <c r="Y51" s="72"/>
       <c r="Z51" s="89" t="s">
@@ -21120,7 +21120,7 @@
         <v>1849</v>
       </c>
       <c r="AB51" s="91" t="s">
-        <v>2010</v>
+        <v>2007</v>
       </c>
       <c r="AC51" s="72"/>
       <c r="AD51" s="89" t="s">
@@ -21130,7 +21130,7 @@
         <v>1849</v>
       </c>
       <c r="AF51" s="91" t="s">
-        <v>2239</v>
+        <v>2228</v>
       </c>
       <c r="AG51" s="72"/>
       <c r="AH51" s="89" t="s">
@@ -21140,7 +21140,7 @@
         <v>1849</v>
       </c>
       <c r="AJ51" s="91" t="s">
-        <v>2245</v>
+        <v>2234</v>
       </c>
       <c r="AK51" s="72"/>
       <c r="AL51" s="89" t="s">
@@ -21150,7 +21150,7 @@
         <v>1849</v>
       </c>
       <c r="AN51" s="91" t="s">
-        <v>2302</v>
+        <v>2288</v>
       </c>
       <c r="AO51" s="72"/>
       <c r="AP51" s="96" t="s">
@@ -21160,7 +21160,7 @@
         <v>1849</v>
       </c>
       <c r="AR51" s="98" t="s">
-        <v>2252</v>
+        <v>2241</v>
       </c>
       <c r="AS51" s="72"/>
       <c r="AT51" s="89"/>
@@ -22985,7 +22985,7 @@
         <v>155</v>
       </c>
       <c r="I10" s="43" t="s">
-        <v>2060</v>
+        <v>2056</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="19.5" customHeight="1">
@@ -23109,7 +23109,7 @@
         <v>206</v>
       </c>
       <c r="F16" s="43" t="s">
-        <v>2070</v>
+        <v>2066</v>
       </c>
       <c r="G16" s="43" t="s">
         <v>210</v>
@@ -23147,7 +23147,7 @@
         <v>224</v>
       </c>
       <c r="F17" s="43" t="s">
-        <v>2071</v>
+        <v>2067</v>
       </c>
       <c r="G17" s="43" t="s">
         <v>228</v>
@@ -23244,7 +23244,7 @@
         <v>284</v>
       </c>
       <c r="J19" s="43" t="s">
-        <v>2040</v>
+        <v>2036</v>
       </c>
       <c r="L19" s="43" t="s">
         <v>289</v>
@@ -23300,7 +23300,7 @@
         <v>318</v>
       </c>
       <c r="O20" s="43" t="s">
-        <v>2075</v>
+        <v>2071</v>
       </c>
       <c r="P20" s="43" t="s">
         <v>320</v>
@@ -23394,7 +23394,7 @@
         <v>380</v>
       </c>
       <c r="J22" s="66" t="s">
-        <v>2061</v>
+        <v>2057</v>
       </c>
       <c r="L22" s="43" t="s">
         <v>382</v>
@@ -23432,10 +23432,10 @@
         <v>395</v>
       </c>
       <c r="C23" s="67" t="s">
-        <v>2068</v>
+        <v>2064</v>
       </c>
       <c r="E23" s="67" t="s">
-        <v>2069</v>
+        <v>2065</v>
       </c>
       <c r="F23" s="43" t="s">
         <v>399</v>
@@ -23468,13 +23468,13 @@
         <v>118</v>
       </c>
       <c r="R23" s="43" t="s">
-        <v>2074</v>
+        <v>2070</v>
       </c>
       <c r="S23" s="43" t="s">
         <v>415</v>
       </c>
       <c r="T23" s="43" t="s">
-        <v>2073</v>
+        <v>2069</v>
       </c>
       <c r="U23" s="43" t="s">
         <v>417</v>
@@ -23497,7 +23497,7 @@
         <v>423</v>
       </c>
       <c r="F24" s="43" t="s">
-        <v>2072</v>
+        <v>2068</v>
       </c>
       <c r="G24" s="43" t="s">
         <v>428</v>
@@ -23550,13 +23550,13 @@
         <v>X</v>
       </c>
       <c r="B25" s="43" t="s">
-        <v>2062</v>
+        <v>2058</v>
       </c>
       <c r="C25" s="43" t="s">
-        <v>2063</v>
+        <v>2059</v>
       </c>
       <c r="E25" s="43" t="s">
-        <v>2064</v>
+        <v>2060</v>
       </c>
       <c r="F25" s="43" t="s">
         <v>461</v>
@@ -23601,13 +23601,13 @@
         <v>481</v>
       </c>
       <c r="V25" s="43" t="s">
-        <v>2065</v>
+        <v>2061</v>
       </c>
       <c r="W25" s="67" t="s">
-        <v>2066</v>
+        <v>2062</v>
       </c>
       <c r="X25" s="67" t="s">
-        <v>2067</v>
+        <v>2063</v>
       </c>
     </row>
     <row r="26" spans="1:24" ht="19.5" customHeight="1">
@@ -24253,7 +24253,7 @@
         <v>127</v>
       </c>
       <c r="C8" s="48" t="s">
-        <v>2057</v>
+        <v>2053</v>
       </c>
       <c r="D8" s="48"/>
       <c r="E8" s="48" t="s">
@@ -24459,7 +24459,7 @@
       </c>
       <c r="D13" s="48"/>
       <c r="E13" s="48" t="s">
-        <v>2027</v>
+        <v>2023</v>
       </c>
       <c r="F13" s="48" t="s">
         <v>185</v>
@@ -24468,7 +24468,7 @@
         <v>115</v>
       </c>
       <c r="H13" s="48" t="s">
-        <v>2059</v>
+        <v>2055</v>
       </c>
       <c r="I13" s="48" t="s">
         <v>187</v>
@@ -24560,13 +24560,13 @@
         <v>217</v>
       </c>
       <c r="F15" s="48" t="s">
-        <v>2011</v>
+        <v>2008</v>
       </c>
       <c r="G15" s="48" t="s">
         <v>221</v>
       </c>
       <c r="H15" s="48" t="s">
-        <v>2038</v>
+        <v>2034</v>
       </c>
       <c r="I15" s="48" t="s">
         <v>225</v>
@@ -24609,7 +24609,7 @@
       </c>
       <c r="D16" s="48"/>
       <c r="E16" s="48" t="s">
-        <v>2056</v>
+        <v>2052</v>
       </c>
       <c r="F16" s="48" t="s">
         <v>251</v>
@@ -24728,7 +24728,7 @@
         <v>326</v>
       </c>
       <c r="H18" s="48" t="s">
-        <v>2029</v>
+        <v>2025</v>
       </c>
       <c r="I18" s="48" t="s">
         <v>332</v>
@@ -24744,7 +24744,7 @@
         <v>342</v>
       </c>
       <c r="N18" s="64" t="s">
-        <v>2020</v>
+        <v>2016</v>
       </c>
       <c r="O18" s="48" t="s">
         <v>347</v>
@@ -24777,7 +24777,7 @@
       </c>
       <c r="D19" s="48"/>
       <c r="E19" s="48" t="s">
-        <v>2058</v>
+        <v>2054</v>
       </c>
       <c r="F19" s="48" t="s">
         <v>366</v>
@@ -24808,7 +24808,7 @@
         <v>379</v>
       </c>
       <c r="P19" s="48" t="s">
-        <v>2035</v>
+        <v>2031</v>
       </c>
       <c r="Q19" s="48" t="s">
         <v>381</v>
@@ -25022,20 +25022,20 @@
         <v>V</v>
       </c>
       <c r="B23" s="48" t="s">
-        <v>2018</v>
+        <v>2014</v>
       </c>
       <c r="C23" s="48" t="s">
         <v>482</v>
       </c>
       <c r="D23" s="48"/>
       <c r="E23" s="48" t="s">
-        <v>2037</v>
+        <v>2033</v>
       </c>
       <c r="F23" s="48" t="s">
         <v>483</v>
       </c>
       <c r="G23" s="63" t="s">
-        <v>2017</v>
+        <v>2013</v>
       </c>
       <c r="H23" s="48" t="s">
         <v>484</v>
@@ -25048,7 +25048,7 @@
         <v>1857</v>
       </c>
       <c r="L23" s="48" t="s">
-        <v>2019</v>
+        <v>2015</v>
       </c>
       <c r="M23" s="48" t="s">
         <v>487</v>
@@ -25163,7 +25163,7 @@
         <v>515</v>
       </c>
       <c r="C25" s="48" t="s">
-        <v>2036</v>
+        <v>2032</v>
       </c>
       <c r="D25" s="48"/>
       <c r="E25" s="48" t="s">
@@ -25201,10 +25201,10 @@
         <v>524</v>
       </c>
       <c r="Q25" s="48" t="s">
-        <v>2028</v>
+        <v>2024</v>
       </c>
       <c r="R25" s="48" t="s">
-        <v>2030</v>
+        <v>2026</v>
       </c>
       <c r="S25" s="48" t="s">
         <v>525</v>
@@ -25222,7 +25222,7 @@
         <v>528</v>
       </c>
       <c r="X25" s="48" t="s">
-        <v>2039</v>
+        <v>2035</v>
       </c>
       <c r="Y25" s="48"/>
       <c r="Z25" s="48"/>

</xml_diff>